<commit_message>
All Features implemented, psASM first working prototype done.
</commit_message>
<xml_diff>
--- a/Doc/Encodings.xlsx
+++ b/Doc/Encodings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pschilk\home\Repos\psMCU\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1209F46-643F-476D-9B0C-1F0CF7081894}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1058428E-0767-4FB8-9438-A6B6D9ED57C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="8820" windowHeight="5748" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inst Decoding" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="101">
   <si>
     <t>Operation</t>
   </si>
@@ -200,9 +200,6 @@
     <t>skip8-16</t>
   </si>
   <si>
-    <t>KOMP B -&gt; B</t>
-  </si>
-  <si>
     <t>0x0E,0x0F</t>
   </si>
   <si>
@@ -287,40 +284,52 @@
     <t>[AND/OR/XOR](L)</t>
   </si>
   <si>
-    <t>WT[A/B]</t>
-  </si>
-  <si>
-    <t>RD[A/B]</t>
-  </si>
-  <si>
     <t>SHFT[R/L](L)</t>
   </si>
   <si>
     <t>ADD(L)</t>
   </si>
   <si>
-    <t>WTD</t>
-  </si>
-  <si>
-    <t>RDD</t>
-  </si>
-  <si>
     <t>CPY</t>
   </si>
   <si>
     <t>NOTA</t>
   </si>
   <si>
-    <t>KOMPB</t>
-  </si>
-  <si>
     <t>SUB</t>
   </si>
   <si>
     <t>SWP</t>
   </si>
   <si>
-    <t>LIT[A/B]</t>
+    <t>SV[A/B]</t>
+  </si>
+  <si>
+    <t>LD[A/B]</t>
+  </si>
+  <si>
+    <t>LIT</t>
+  </si>
+  <si>
+    <t>SVD[P/M]</t>
+  </si>
+  <si>
+    <t>LDD[P/M]</t>
+  </si>
+  <si>
+    <t>A=0</t>
+  </si>
+  <si>
+    <t>B=0</t>
+  </si>
+  <si>
+    <t>A=B</t>
+  </si>
+  <si>
+    <t>COMP B -&gt; B</t>
+  </si>
+  <si>
+    <t>COMPB</t>
   </si>
 </sst>
 </file>
@@ -602,6 +611,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -624,15 +642,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1135,14 +1144,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59778E2C-D2B8-41E1-8336-5F65E1F1812B}">
   <dimension ref="A1:R23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.33203125" customWidth="1"/>
-    <col min="2" max="2" width="16.77734375" style="28" customWidth="1"/>
+    <col min="2" max="2" width="16.77734375" style="20" customWidth="1"/>
     <col min="10" max="10" width="11.109375" style="16" customWidth="1"/>
     <col min="11" max="11" width="13.88671875" style="16" customWidth="1"/>
     <col min="12" max="18" width="8.88671875" style="16"/>
@@ -1152,8 +1161,8 @@
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="26" t="s">
-        <v>80</v>
+      <c r="B1" s="18" t="s">
+        <v>79</v>
       </c>
       <c r="C1" s="2">
         <v>15</v>
@@ -1196,8 +1205,8 @@
       <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="27" t="s">
-        <v>81</v>
+      <c r="B2" s="19" t="s">
+        <v>80</v>
       </c>
       <c r="C2" s="6">
         <v>1</v>
@@ -1205,18 +1214,18 @@
       <c r="D2" s="7">
         <v>1</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
       <c r="J2" s="14" t="s">
         <v>55</v>
       </c>
       <c r="K2" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L2" s="14">
         <v>32</v>
@@ -1232,8 +1241,8 @@
       <c r="A3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="28" t="s">
-        <v>82</v>
+      <c r="B3" s="20" t="s">
+        <v>81</v>
       </c>
       <c r="C3" s="9">
         <v>1</v>
@@ -1241,18 +1250,18 @@
       <c r="D3" s="9">
         <v>0</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
       <c r="J3" s="14" t="s">
         <v>54</v>
       </c>
       <c r="K3" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L3" s="14">
         <v>32</v>
@@ -1268,8 +1277,8 @@
       <c r="A4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="28" t="s">
-        <v>83</v>
+      <c r="B4" s="20" t="s">
+        <v>82</v>
       </c>
       <c r="C4" s="9">
         <v>0</v>
@@ -1283,16 +1292,16 @@
       <c r="F4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="22" t="s">
+      <c r="G4" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
       <c r="J4" s="14" t="s">
         <v>53</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L4" s="14">
         <v>16</v>
@@ -1308,8 +1317,8 @@
       <c r="A5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="28" t="s">
-        <v>84</v>
+      <c r="B5" s="20" t="s">
+        <v>83</v>
       </c>
       <c r="C5" s="9">
         <v>0</v>
@@ -1323,11 +1332,11 @@
       <c r="F5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="22" t="s">
+      <c r="G5" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
       <c r="J5" s="14" t="s">
         <v>52</v>
       </c>
@@ -1348,8 +1357,8 @@
       <c r="A6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="28" t="s">
-        <v>85</v>
+      <c r="B6" s="20" t="s">
+        <v>84</v>
       </c>
       <c r="C6" s="9">
         <v>0</v>
@@ -1366,10 +1375,10 @@
       <c r="G6" s="7">
         <v>1</v>
       </c>
-      <c r="H6" s="23" t="s">
+      <c r="H6" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="I6" s="23"/>
+      <c r="I6" s="26"/>
       <c r="J6" s="14" t="s">
         <v>47</v>
       </c>
@@ -1390,8 +1399,8 @@
       <c r="A7" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="28" t="s">
-        <v>86</v>
+      <c r="B7" s="20" t="s">
+        <v>91</v>
       </c>
       <c r="C7" s="9">
         <v>0</v>
@@ -1415,10 +1424,10 @@
         <v>18</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L7" s="14">
         <v>2</v>
@@ -1434,8 +1443,8 @@
       <c r="A8" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="28" t="s">
-        <v>87</v>
+      <c r="B8" s="20" t="s">
+        <v>92</v>
       </c>
       <c r="C8" s="9">
         <v>0</v>
@@ -1459,10 +1468,10 @@
         <v>18</v>
       </c>
       <c r="J8" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K8" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L8" s="14">
         <v>2</v>
@@ -1478,8 +1487,8 @@
       <c r="A9" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="28" t="s">
-        <v>97</v>
+      <c r="B9" s="20" t="s">
+        <v>93</v>
       </c>
       <c r="C9" s="9">
         <v>0</v>
@@ -1503,10 +1512,10 @@
         <v>18</v>
       </c>
       <c r="J9" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L9" s="14">
         <v>2</v>
@@ -1522,8 +1531,8 @@
       <c r="A10" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="28" t="s">
-        <v>88</v>
+      <c r="B10" s="20" t="s">
+        <v>85</v>
       </c>
       <c r="C10" s="9">
         <v>0</v>
@@ -1566,8 +1575,8 @@
       <c r="A11" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="28" t="s">
-        <v>89</v>
+      <c r="B11" s="20" t="s">
+        <v>86</v>
       </c>
       <c r="C11" s="9">
         <v>0</v>
@@ -1610,8 +1619,8 @@
       <c r="A12" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="28" t="s">
-        <v>90</v>
+      <c r="B12" s="20" t="s">
+        <v>94</v>
       </c>
       <c r="C12" s="9">
         <v>0</v>
@@ -1654,8 +1663,8 @@
       <c r="A13" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="28" t="s">
-        <v>91</v>
+      <c r="B13" s="20" t="s">
+        <v>95</v>
       </c>
       <c r="C13" s="9">
         <v>0</v>
@@ -1696,10 +1705,10 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14" s="28" t="s">
-        <v>92</v>
+        <v>60</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>87</v>
       </c>
       <c r="C14" s="9">
         <v>0</v>
@@ -1742,8 +1751,8 @@
       <c r="A15" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="28" t="s">
-        <v>93</v>
+      <c r="B15" s="20" t="s">
+        <v>88</v>
       </c>
       <c r="C15" s="9">
         <v>0</v>
@@ -1784,10 +1793,10 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B16" s="28" t="s">
-        <v>94</v>
+        <v>99</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>100</v>
       </c>
       <c r="C16" s="9">
         <v>0</v>
@@ -1830,8 +1839,8 @@
       <c r="A17" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="28" t="s">
-        <v>95</v>
+      <c r="B17" s="20" t="s">
+        <v>89</v>
       </c>
       <c r="C17" s="9">
         <v>0</v>
@@ -1874,7 +1883,7 @@
       <c r="A18" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="20" t="s">
         <v>26</v>
       </c>
       <c r="C18" s="9">
@@ -1918,7 +1927,7 @@
       <c r="A19" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="20" t="s">
         <v>27</v>
       </c>
       <c r="C19" s="9">
@@ -1962,7 +1971,7 @@
       <c r="A20" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="20" t="s">
         <v>28</v>
       </c>
       <c r="C20" s="9">
@@ -2006,8 +2015,8 @@
       <c r="A21" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="28" t="s">
-        <v>96</v>
+      <c r="B21" s="20" t="s">
+        <v>90</v>
       </c>
       <c r="C21" s="9">
         <v>0</v>
@@ -2050,7 +2059,7 @@
       <c r="A22" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="20" t="s">
         <v>30</v>
       </c>
       <c r="C22" s="9">
@@ -2094,7 +2103,7 @@
       <c r="A23" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="28" t="s">
+      <c r="B23" s="20" t="s">
         <v>31</v>
       </c>
       <c r="C23" s="9">
@@ -2287,10 +2296,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="24"/>
+      <c r="A1" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="27"/>
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -2352,7 +2361,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="A1:H4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2362,20 +2371,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
+      <c r="A1" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B2" s="7">
         <v>6</v>
@@ -2396,76 +2405,76 @@
         <v>1</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="7">
-        <v>0</v>
-      </c>
-      <c r="B3" s="7">
-        <v>0</v>
-      </c>
-      <c r="C3" s="7">
-        <v>0</v>
+      <c r="A3" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>96</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>78</v>
-      </c>
       <c r="E4" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
+      <c r="A7" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B8" s="7">
         <v>6</v>
@@ -2486,7 +2495,7 @@
         <v>1</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -2502,37 +2511,37 @@
       <c r="D9" s="7">
         <v>0</v>
       </c>
-      <c r="E9" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
+      <c r="E9" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="F10" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="G10" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="H10" s="7" t="s">
         <v>77</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed System Registers, Updated Doc
</commit_message>
<xml_diff>
--- a/Doc/Encodings.xlsx
+++ b/Doc/Encodings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pschilk\home\Repos\psMCU\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B4BD39-8814-49E4-B3C6-33F42E7E2CBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D44D541A-6AC5-4F71-839B-0735FFCD67DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inst Decoding" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="109">
   <si>
     <t>Operation</t>
   </si>
@@ -227,9 +227,6 @@
     <t>0x18</t>
   </si>
   <si>
-    <t>Status Reg (Adr 0x100)</t>
-  </si>
-  <si>
     <t>7 (MSB)</t>
   </si>
   <si>
@@ -326,15 +323,9 @@
     <t>COMPB</t>
   </si>
   <si>
-    <t>Config Reg (Adr 0x101)</t>
-  </si>
-  <si>
     <t>INT_EN</t>
   </si>
   <si>
-    <t>INT Reg (Adr 0x102)</t>
-  </si>
-  <si>
     <t>RTRNI</t>
   </si>
   <si>
@@ -348,6 +339,21 @@
   </si>
   <si>
     <t>skip7-16</t>
+  </si>
+  <si>
+    <t>System Reg 1 (Adr 0x100)</t>
+  </si>
+  <si>
+    <t>System Reg 2 (Adr 0x101)</t>
+  </si>
+  <si>
+    <t>System Reg 3 (Adr 0x102)</t>
+  </si>
+  <si>
+    <t>A&gt;B</t>
+  </si>
+  <si>
+    <t>B&lt;A</t>
   </si>
 </sst>
 </file>
@@ -599,7 +605,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -661,6 +667,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1215,7 +1224,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59778E2C-D2B8-41E1-8336-5F65E1F1812B}">
   <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
@@ -1233,7 +1242,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C1" s="2">
         <v>15</v>
@@ -1277,7 +1286,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C2" s="6">
         <v>1</v>
@@ -1285,18 +1294,18 @@
       <c r="D2" s="7">
         <v>1</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
       <c r="J2" s="14" t="s">
         <v>55</v>
       </c>
       <c r="K2" s="14" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="L2" s="14">
         <v>32</v>
@@ -1313,7 +1322,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C3" s="9">
         <v>1</v>
@@ -1321,13 +1330,13 @@
       <c r="D3" s="9">
         <v>0</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
       <c r="J3" s="14" t="s">
         <v>54</v>
       </c>
@@ -1349,7 +1358,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C4" s="9">
         <v>0</v>
@@ -1363,11 +1372,11 @@
       <c r="F4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="29" t="s">
+      <c r="G4" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
       <c r="J4" s="14" t="s">
         <v>53</v>
       </c>
@@ -1389,7 +1398,7 @@
         <v>13</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C5" s="9">
         <v>0</v>
@@ -1403,11 +1412,11 @@
       <c r="F5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
       <c r="J5" s="14" t="s">
         <v>52</v>
       </c>
@@ -1415,7 +1424,7 @@
         <v>63</v>
       </c>
       <c r="L5" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="M5" s="14"/>
       <c r="N5" s="14"/>
@@ -1426,10 +1435,10 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C6" s="9">
         <v>0</v>
@@ -1453,7 +1462,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="K6" s="14" t="s">
         <v>50</v>
@@ -1473,7 +1482,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C7" s="9">
         <v>0</v>
@@ -1490,10 +1499,10 @@
       <c r="G7" s="7">
         <v>1</v>
       </c>
-      <c r="H7" s="30" t="s">
+      <c r="H7" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="30"/>
+      <c r="I7" s="31"/>
       <c r="J7" s="14" t="s">
         <v>47</v>
       </c>
@@ -1515,7 +1524,7 @@
         <v>17</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C8" s="9">
         <v>0</v>
@@ -1559,7 +1568,7 @@
         <v>19</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C9" s="9">
         <v>0</v>
@@ -1603,7 +1612,7 @@
         <v>16</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C10" s="9">
         <v>0</v>
@@ -1647,7 +1656,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C11" s="9">
         <v>0</v>
@@ -1691,7 +1700,7 @@
         <v>21</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C12" s="9">
         <v>0</v>
@@ -1735,7 +1744,7 @@
         <v>22</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C13" s="9">
         <v>0</v>
@@ -1779,7 +1788,7 @@
         <v>23</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C14" s="9">
         <v>0</v>
@@ -1823,7 +1832,7 @@
         <v>59</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C15" s="9">
         <v>0</v>
@@ -1867,7 +1876,7 @@
         <v>24</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C16" s="9">
         <v>0</v>
@@ -1908,10 +1917,10 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17" s="20" t="s">
         <v>97</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>98</v>
       </c>
       <c r="C17" s="9">
         <v>0</v>
@@ -1955,7 +1964,7 @@
         <v>25</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C18" s="9">
         <v>0</v>
@@ -2131,7 +2140,7 @@
         <v>29</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C22" s="9">
         <v>0</v>
@@ -2427,10 +2436,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="31"/>
+      <c r="A1" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="32"/>
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -2489,33 +2498,34 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D74D41B-283E-4F55-BA94-91EF2EF7E1E9}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="4" max="4" width="12.88671875" customWidth="1"/>
     <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
+      <c r="A1" s="33" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" s="7">
         <v>6</v>
@@ -2536,76 +2546,76 @@
         <v>1</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>94</v>
+      <c r="A3" s="25">
+        <v>0</v>
+      </c>
+      <c r="B3" s="25">
+        <v>0</v>
+      </c>
+      <c r="C3" s="25">
+        <v>0</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>73</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="32" t="s">
-        <v>99</v>
-      </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
+      <c r="A7" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B8" s="7">
         <v>6</v>
@@ -2626,7 +2636,7 @@
         <v>1</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -2642,132 +2652,132 @@
       <c r="D9" s="7">
         <v>0</v>
       </c>
-      <c r="E9" s="32" t="s">
-        <v>69</v>
-      </c>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
+      <c r="E9" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="F10" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="G10" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="H10" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>75</v>
-      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="B14" s="32"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
+      <c r="A14" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="21">
+        <v>6</v>
+      </c>
+      <c r="C14" s="21">
+        <v>5</v>
+      </c>
+      <c r="D14" s="21">
+        <v>4</v>
+      </c>
+      <c r="E14" s="21">
+        <v>3</v>
+      </c>
+      <c r="F14" s="21">
+        <v>2</v>
+      </c>
+      <c r="G14" s="21">
+        <v>1</v>
+      </c>
+      <c r="H14" s="21" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="21" t="s">
-        <v>67</v>
+      <c r="A15" s="21">
+        <v>0</v>
       </c>
       <c r="B15" s="21">
-        <v>6</v>
-      </c>
-      <c r="C15" s="21">
-        <v>5</v>
-      </c>
-      <c r="D15" s="21">
-        <v>4</v>
-      </c>
-      <c r="E15" s="21">
-        <v>3</v>
-      </c>
-      <c r="F15" s="21">
-        <v>2</v>
-      </c>
-      <c r="G15" s="21">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>93</v>
       </c>
       <c r="H15" s="21" t="s">
-        <v>68</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="21">
-        <v>0</v>
-      </c>
-      <c r="B16" s="21">
-        <v>0</v>
-      </c>
-      <c r="C16" s="21">
-        <v>0</v>
-      </c>
-      <c r="D16" s="21">
-        <v>0</v>
-      </c>
-      <c r="E16" s="21">
-        <v>0</v>
-      </c>
-      <c r="F16" s="21">
-        <v>0</v>
-      </c>
-      <c r="G16" s="21">
-        <v>0</v>
+      <c r="A16" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="G16" s="21" t="s">
+        <v>73</v>
       </c>
       <c r="H16" s="21" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="21" t="s">
         <v>74</v>
-      </c>
-      <c r="B17" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="C17" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="D17" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="E17" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="F17" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="G17" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="H17" s="21" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="A13:H13"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A7:H7"/>
     <mergeCell ref="E9:H9"/>

</xml_diff>

<commit_message>
Cleaned up Programms, Updated some Documentation.
</commit_message>
<xml_diff>
--- a/Doc/Encodings.xlsx
+++ b/Doc/Encodings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pschilk\home\Repos\psMCU\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D44D541A-6AC5-4F71-839B-0735FFCD67DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD682B8-4ABC-4BC2-AFBA-4607C26340EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inst Decoding" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="114">
   <si>
     <t>Operation</t>
   </si>
@@ -62,9 +62,6 @@
     <t>TestBitRAM</t>
   </si>
   <si>
-    <t>1/0</t>
-  </si>
-  <si>
     <t>Bit</t>
   </si>
   <si>
@@ -341,19 +338,37 @@
     <t>skip7-16</t>
   </si>
   <si>
-    <t>System Reg 1 (Adr 0x100)</t>
-  </si>
-  <si>
-    <t>System Reg 2 (Adr 0x101)</t>
-  </si>
-  <si>
-    <t>System Reg 3 (Adr 0x102)</t>
-  </si>
-  <si>
     <t>A&gt;B</t>
   </si>
   <si>
     <t>B&lt;A</t>
+  </si>
+  <si>
+    <t>Scratch Reg 1 (Adr 0x100)</t>
+  </si>
+  <si>
+    <t>Scratch Reg 1</t>
+  </si>
+  <si>
+    <t>Scratch Reg 2 (Adr 0x101)</t>
+  </si>
+  <si>
+    <t>Scratch Reg 3 (Adr 0x102)</t>
+  </si>
+  <si>
+    <t>Scratch Reg 4 (Adr 0x103)</t>
+  </si>
+  <si>
+    <t>System Reg 1 (Adr 0x104)</t>
+  </si>
+  <si>
+    <t>System Reg 2 (Adr 0x105)</t>
+  </si>
+  <si>
+    <t>System Reg 3 (Adr 0x106)</t>
+  </si>
+  <si>
+    <t>Skip if 1/0</t>
   </si>
 </sst>
 </file>
@@ -605,7 +620,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -672,6 +687,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -694,6 +712,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1224,8 +1251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59778E2C-D2B8-41E1-8336-5F65E1F1812B}">
   <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1242,7 +1269,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C1" s="2">
         <v>15</v>
@@ -1266,13 +1293,13 @@
         <v>9</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L1" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M1" s="14"/>
       <c r="N1" s="14"/>
@@ -1286,7 +1313,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C2" s="6">
         <v>1</v>
@@ -1294,18 +1321,18 @@
       <c r="D2" s="7">
         <v>1</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
       <c r="J2" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K2" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L2" s="14">
         <v>32</v>
@@ -1322,7 +1349,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C3" s="9">
         <v>1</v>
@@ -1330,18 +1357,18 @@
       <c r="D3" s="9">
         <v>0</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
       <c r="J3" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K3" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L3" s="14">
         <v>32</v>
@@ -1358,7 +1385,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C4" s="9">
         <v>0</v>
@@ -1370,18 +1397,18 @@
         <v>1</v>
       </c>
       <c r="F4" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="G4" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
       <c r="J4" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L4" s="14">
         <v>16</v>
@@ -1395,10 +1422,10 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C5" s="9">
         <v>0</v>
@@ -1410,21 +1437,21 @@
         <v>0</v>
       </c>
       <c r="F5" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="G5" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
       <c r="J5" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K5" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L5" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M5" s="14"/>
       <c r="N5" s="14"/>
@@ -1435,37 +1462,37 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" s="9">
+        <v>0</v>
+      </c>
+      <c r="D6" s="23">
+        <v>0</v>
+      </c>
+      <c r="E6" s="24">
+        <v>1</v>
+      </c>
+      <c r="F6" s="10">
+        <v>1</v>
+      </c>
+      <c r="G6" s="22">
+        <v>0</v>
+      </c>
+      <c r="H6" s="22">
+        <v>0</v>
+      </c>
+      <c r="I6" s="22">
+        <v>0</v>
+      </c>
+      <c r="J6" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="B6" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="C6" s="9">
-        <v>0</v>
-      </c>
-      <c r="D6" s="23">
-        <v>0</v>
-      </c>
-      <c r="E6" s="24">
-        <v>1</v>
-      </c>
-      <c r="F6" s="10">
-        <v>1</v>
-      </c>
-      <c r="G6" s="22">
-        <v>0</v>
-      </c>
-      <c r="H6" s="22">
-        <v>0</v>
-      </c>
-      <c r="I6" s="22">
-        <v>0</v>
-      </c>
-      <c r="J6" s="14" t="s">
-        <v>101</v>
-      </c>
       <c r="K6" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L6" s="14">
         <v>1</v>
@@ -1479,35 +1506,35 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" s="9">
+        <v>0</v>
+      </c>
+      <c r="D7" s="7">
+        <v>0</v>
+      </c>
+      <c r="E7" s="7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="7">
+        <v>0</v>
+      </c>
+      <c r="G7" s="7">
+        <v>1</v>
+      </c>
+      <c r="H7" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="C7" s="9">
-        <v>0</v>
-      </c>
-      <c r="D7" s="7">
-        <v>0</v>
-      </c>
-      <c r="E7" s="7">
-        <v>1</v>
-      </c>
-      <c r="F7" s="7">
-        <v>0</v>
-      </c>
-      <c r="G7" s="7">
-        <v>1</v>
-      </c>
-      <c r="H7" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="31"/>
+      <c r="I7" s="32"/>
       <c r="J7" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L7" s="14">
         <v>4</v>
@@ -1521,37 +1548,37 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="9">
+        <v>0</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0</v>
+      </c>
+      <c r="E8" s="7">
+        <v>1</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0</v>
+      </c>
+      <c r="G8" s="7">
+        <v>0</v>
+      </c>
+      <c r="H8" s="7">
+        <v>1</v>
+      </c>
+      <c r="I8" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="C8" s="9">
-        <v>0</v>
-      </c>
-      <c r="D8" s="7">
-        <v>0</v>
-      </c>
-      <c r="E8" s="7">
-        <v>1</v>
-      </c>
-      <c r="F8" s="7">
-        <v>0</v>
-      </c>
-      <c r="G8" s="7">
-        <v>0</v>
-      </c>
-      <c r="H8" s="7">
-        <v>1</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>18</v>
-      </c>
       <c r="J8" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K8" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L8" s="14">
         <v>2</v>
@@ -1565,10 +1592,10 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C9" s="9">
         <v>0</v>
@@ -1589,13 +1616,13 @@
         <v>0</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L9" s="14">
         <v>2</v>
@@ -1609,10 +1636,10 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C10" s="9">
         <v>0</v>
@@ -1633,13 +1660,13 @@
         <v>1</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J10" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K10" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L10" s="14">
         <v>2</v>
@@ -1653,10 +1680,10 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C11" s="9">
         <v>0</v>
@@ -1680,10 +1707,10 @@
         <v>1</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K11" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L11" s="14">
         <v>1</v>
@@ -1697,10 +1724,10 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C12" s="9">
         <v>0</v>
@@ -1724,10 +1751,10 @@
         <v>0</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K12" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L12" s="14">
         <v>1</v>
@@ -1741,10 +1768,10 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C13" s="9">
         <v>0</v>
@@ -1768,10 +1795,10 @@
         <v>1</v>
       </c>
       <c r="J13" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K13" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L13" s="14">
         <v>1</v>
@@ -1785,10 +1812,10 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C14" s="9">
         <v>0</v>
@@ -1812,10 +1839,10 @@
         <v>0</v>
       </c>
       <c r="J14" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K14" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L14" s="14">
         <v>1</v>
@@ -1829,10 +1856,10 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C15" s="9">
         <v>0</v>
@@ -1856,10 +1883,10 @@
         <v>1</v>
       </c>
       <c r="J15" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K15" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L15" s="14">
         <v>1</v>
@@ -1873,10 +1900,10 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C16" s="9">
         <v>0</v>
@@ -1900,10 +1927,10 @@
         <v>0</v>
       </c>
       <c r="J16" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K16" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L16" s="14">
         <v>1</v>
@@ -1917,11 +1944,11 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B17" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="B17" s="20" t="s">
-        <v>97</v>
-      </c>
       <c r="C17" s="9">
         <v>0</v>
       </c>
@@ -1944,10 +1971,10 @@
         <v>1</v>
       </c>
       <c r="J17" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K17" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L17" s="14">
         <v>1</v>
@@ -1961,10 +1988,10 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C18" s="9">
         <v>0</v>
@@ -1988,10 +2015,10 @@
         <v>0</v>
       </c>
       <c r="J18" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K18" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L18" s="14">
         <v>1</v>
@@ -2005,10 +2032,10 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C19" s="9">
         <v>0</v>
@@ -2032,10 +2059,10 @@
         <v>1</v>
       </c>
       <c r="J19" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K19" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L19" s="14">
         <v>1</v>
@@ -2049,10 +2076,10 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C20" s="9">
         <v>0</v>
@@ -2076,10 +2103,10 @@
         <v>0</v>
       </c>
       <c r="J20" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K20" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L20" s="14">
         <v>1</v>
@@ -2093,10 +2120,10 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C21" s="9">
         <v>0</v>
@@ -2120,10 +2147,10 @@
         <v>1</v>
       </c>
       <c r="J21" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K21" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L21" s="14">
         <v>1</v>
@@ -2137,10 +2164,10 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C22" s="9">
         <v>0</v>
@@ -2164,10 +2191,10 @@
         <v>0</v>
       </c>
       <c r="J22" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K22" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L22" s="14">
         <v>1</v>
@@ -2181,10 +2208,10 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C23" s="9">
         <v>0</v>
@@ -2208,10 +2235,10 @@
         <v>1</v>
       </c>
       <c r="J23" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K23" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L23" s="14">
         <v>1</v>
@@ -2225,10 +2252,10 @@
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C24" s="9">
         <v>0</v>
@@ -2252,10 +2279,10 @@
         <v>0</v>
       </c>
       <c r="J24" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K24" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L24" s="14">
         <v>1</v>
@@ -2275,7 +2302,7 @@
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="H7:I7"/>
   </mergeCells>
-  <conditionalFormatting sqref="C3 C12:C24 E12:I24 C8:I11 C7:H7 C5:D6 F5:F6 D4:G4 C2:E2">
+  <conditionalFormatting sqref="C3 C12:C24 E12:I24 C8:I11 C7:H7 C5:D6 F5:F6 C2:E2 D4:G4">
     <cfRule type="cellIs" dxfId="34" priority="52" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -2331,7 +2358,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7:I24 C5:D6 C1:I1 C4:I4 C3 E3 C2:E2 F5:I6">
+  <conditionalFormatting sqref="C7:I24 C5:D6 C1:I1 C3 E3 C2:E2 F5:I6 C4:I4">
     <cfRule type="containsText" dxfId="20" priority="21" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",C1)))</formula>
     </cfRule>
@@ -2436,10 +2463,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="32"/>
+      <c r="A1" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="33"/>
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -2498,10 +2525,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D74D41B-283E-4F55-BA94-91EF2EF7E1E9}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2512,275 +2539,587 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="26">
+        <v>6</v>
+      </c>
+      <c r="C2" s="26">
+        <v>5</v>
+      </c>
+      <c r="D2" s="26">
+        <v>4</v>
+      </c>
+      <c r="E2" s="26">
+        <v>3</v>
+      </c>
+      <c r="F2" s="26">
+        <v>2</v>
+      </c>
+      <c r="G2" s="26">
+        <v>1</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="37"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="H4" s="26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="26">
+        <v>6</v>
+      </c>
+      <c r="C8" s="26">
+        <v>5</v>
+      </c>
+      <c r="D8" s="26">
+        <v>4</v>
+      </c>
+      <c r="E8" s="26">
+        <v>3</v>
+      </c>
+      <c r="F8" s="26">
+        <v>2</v>
+      </c>
+      <c r="G8" s="26">
+        <v>1</v>
+      </c>
+      <c r="H8" s="26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="37"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="G10" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="H10" s="26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="26">
+        <v>6</v>
+      </c>
+      <c r="C14" s="26">
+        <v>5</v>
+      </c>
+      <c r="D14" s="26">
+        <v>4</v>
+      </c>
+      <c r="E14" s="26">
+        <v>3</v>
+      </c>
+      <c r="F14" s="26">
+        <v>2</v>
+      </c>
+      <c r="G14" s="26">
+        <v>1</v>
+      </c>
+      <c r="H14" s="26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="B15" s="36"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="37"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="G16" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="H16" s="26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="B19" s="34"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" s="26">
+        <v>6</v>
+      </c>
+      <c r="C20" s="26">
+        <v>5</v>
+      </c>
+      <c r="D20" s="26">
+        <v>4</v>
+      </c>
+      <c r="E20" s="26">
+        <v>3</v>
+      </c>
+      <c r="F20" s="26">
+        <v>2</v>
+      </c>
+      <c r="G20" s="26">
+        <v>1</v>
+      </c>
+      <c r="H20" s="26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="B21" s="36"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="37"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="F22" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="G22" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="H22" s="26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="B25" s="34"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" s="7">
+        <v>6</v>
+      </c>
+      <c r="C26" s="7">
+        <v>5</v>
+      </c>
+      <c r="D26" s="7">
+        <v>4</v>
+      </c>
+      <c r="E26" s="7">
+        <v>3</v>
+      </c>
+      <c r="F26" s="7">
+        <v>2</v>
+      </c>
+      <c r="G26" s="7">
+        <v>1</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="25">
+        <v>0</v>
+      </c>
+      <c r="B27" s="25">
+        <v>0</v>
+      </c>
+      <c r="C27" s="25">
+        <v>0</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E28" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="B31" s="34"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="34"/>
+      <c r="H31" s="34"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" s="7">
+        <v>6</v>
+      </c>
+      <c r="C32" s="7">
+        <v>5</v>
+      </c>
+      <c r="D32" s="7">
+        <v>4</v>
+      </c>
+      <c r="E32" s="7">
+        <v>3</v>
+      </c>
+      <c r="F32" s="7">
+        <v>2</v>
+      </c>
+      <c r="G32" s="7">
+        <v>1</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="7">
+        <v>0</v>
+      </c>
+      <c r="B33" s="7">
+        <v>0</v>
+      </c>
+      <c r="C33" s="7">
+        <v>0</v>
+      </c>
+      <c r="D33" s="7">
+        <v>0</v>
+      </c>
+      <c r="E33" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="F33" s="34"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="34"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="B37" s="34"/>
+      <c r="C37" s="34"/>
+      <c r="D37" s="34"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
+      <c r="G37" s="34"/>
+      <c r="H37" s="34"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38" s="21">
+        <v>6</v>
+      </c>
+      <c r="C38" s="21">
+        <v>5</v>
+      </c>
+      <c r="D38" s="21">
+        <v>4</v>
+      </c>
+      <c r="E38" s="21">
+        <v>3</v>
+      </c>
+      <c r="F38" s="21">
+        <v>2</v>
+      </c>
+      <c r="G38" s="21">
+        <v>1</v>
+      </c>
+      <c r="H38" s="21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" s="21">
+        <v>0</v>
+      </c>
+      <c r="B39" s="21">
+        <v>0</v>
+      </c>
+      <c r="C39" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="D39" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B2" s="7">
-        <v>6</v>
-      </c>
-      <c r="C2" s="7">
-        <v>5</v>
-      </c>
-      <c r="D2" s="7">
-        <v>4</v>
-      </c>
-      <c r="E2" s="7">
-        <v>3</v>
-      </c>
-      <c r="F2" s="7">
-        <v>2</v>
-      </c>
-      <c r="G2" s="7">
-        <v>1</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="25">
-        <v>0</v>
-      </c>
-      <c r="B3" s="25">
-        <v>0</v>
-      </c>
-      <c r="C3" s="25">
-        <v>0</v>
-      </c>
-      <c r="D3" s="7" t="s">
+      <c r="E39" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="H39" s="21" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E4" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="33" t="s">
-        <v>105</v>
-      </c>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B8" s="7">
-        <v>6</v>
-      </c>
-      <c r="C8" s="7">
-        <v>5</v>
-      </c>
-      <c r="D8" s="7">
-        <v>4</v>
-      </c>
-      <c r="E8" s="7">
-        <v>3</v>
-      </c>
-      <c r="F8" s="7">
-        <v>2</v>
-      </c>
-      <c r="G8" s="7">
-        <v>1</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="7">
-        <v>0</v>
-      </c>
-      <c r="B9" s="7">
-        <v>0</v>
-      </c>
-      <c r="C9" s="7">
-        <v>0</v>
-      </c>
-      <c r="D9" s="7">
-        <v>0</v>
-      </c>
-      <c r="E9" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="33" t="s">
-        <v>106</v>
-      </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="B14" s="21">
-        <v>6</v>
-      </c>
-      <c r="C14" s="21">
-        <v>5</v>
-      </c>
-      <c r="D14" s="21">
-        <v>4</v>
-      </c>
-      <c r="E14" s="21">
-        <v>3</v>
-      </c>
-      <c r="F14" s="21">
-        <v>2</v>
-      </c>
-      <c r="G14" s="21">
-        <v>1</v>
-      </c>
-      <c r="H14" s="21" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="21">
-        <v>0</v>
-      </c>
-      <c r="B15" s="21">
-        <v>0</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="D15" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="H15" s="21" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="C16" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="D16" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="E16" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="F16" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="G16" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="H16" s="21" t="s">
-        <v>74</v>
+      <c r="B40" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="D40" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="E40" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="F40" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="G40" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="H40" s="21" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A13:H13"/>
+  <mergeCells count="12">
+    <mergeCell ref="A37:H37"/>
+    <mergeCell ref="A25:H25"/>
+    <mergeCell ref="A31:H31"/>
+    <mergeCell ref="E33:H33"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A7:H7"/>
-    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="A21:H21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Renamed Conditional and DynamicMem Instructions
</commit_message>
<xml_diff>
--- a/Doc/Encodings.xlsx
+++ b/Doc/Encodings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pschilk\home\Repos\psMCU\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD682B8-4ABC-4BC2-AFBA-4607C26340EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E92272-378F-4719-A9AE-89D41E398D38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36075" yWindow="1695" windowWidth="17040" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inst Decoding" sheetId="2" r:id="rId1"/>
@@ -263,12 +263,6 @@
     <t>CALL</t>
   </si>
   <si>
-    <t>TB[S/R]M</t>
-  </si>
-  <si>
-    <t>TB[S/R]R</t>
-  </si>
-  <si>
     <t>[AND/OR/XOR](L)</t>
   </si>
   <si>
@@ -299,12 +293,6 @@
     <t>LIT</t>
   </si>
   <si>
-    <t>SVD[P/M]</t>
-  </si>
-  <si>
-    <t>LDD[P/M]</t>
-  </si>
-  <si>
     <t>A=0</t>
   </si>
   <si>
@@ -369,6 +357,18 @@
   </si>
   <si>
     <t>Skip if 1/0</t>
+  </si>
+  <si>
+    <t>IF[S/R]M</t>
+  </si>
+  <si>
+    <t>IF[S/R]A</t>
+  </si>
+  <si>
+    <t>SVD[P/R]</t>
+  </si>
+  <si>
+    <t>LDD[P/R]</t>
   </si>
 </sst>
 </file>
@@ -1252,7 +1252,7 @@
   <dimension ref="A1:R24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1332,7 +1332,7 @@
         <v>54</v>
       </c>
       <c r="K2" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="L2" s="14">
         <v>32</v>
@@ -1385,7 +1385,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>78</v>
+        <v>110</v>
       </c>
       <c r="C4" s="9">
         <v>0</v>
@@ -1397,7 +1397,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G4" s="31" t="s">
         <v>11</v>
@@ -1425,7 +1425,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>79</v>
+        <v>111</v>
       </c>
       <c r="C5" s="9">
         <v>0</v>
@@ -1437,7 +1437,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G5" s="31" t="s">
         <v>11</v>
@@ -1451,7 +1451,7 @@
         <v>62</v>
       </c>
       <c r="L5" s="14" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="M5" s="14"/>
       <c r="N5" s="14"/>
@@ -1462,10 +1462,10 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C6" s="9">
         <v>0</v>
@@ -1489,7 +1489,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="K6" s="14" t="s">
         <v>49</v>
@@ -1509,7 +1509,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C7" s="9">
         <v>0</v>
@@ -1551,7 +1551,7 @@
         <v>16</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C8" s="9">
         <v>0</v>
@@ -1595,7 +1595,7 @@
         <v>18</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C9" s="9">
         <v>0</v>
@@ -1639,7 +1639,7 @@
         <v>15</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C10" s="9">
         <v>0</v>
@@ -1683,7 +1683,7 @@
         <v>19</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C11" s="9">
         <v>0</v>
@@ -1727,7 +1727,7 @@
         <v>20</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C12" s="9">
         <v>0</v>
@@ -1771,7 +1771,7 @@
         <v>21</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="C13" s="9">
         <v>0</v>
@@ -1815,7 +1815,7 @@
         <v>22</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="C14" s="9">
         <v>0</v>
@@ -1859,7 +1859,7 @@
         <v>58</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C15" s="9">
         <v>0</v>
@@ -1903,7 +1903,7 @@
         <v>23</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C16" s="9">
         <v>0</v>
@@ -1944,10 +1944,10 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C17" s="9">
         <v>0</v>
@@ -1991,7 +1991,7 @@
         <v>24</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C18" s="9">
         <v>0</v>
@@ -2167,7 +2167,7 @@
         <v>28</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C22" s="9">
         <v>0</v>
@@ -2540,7 +2540,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="34" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B1" s="34"/>
       <c r="C1" s="34"/>
@@ -2578,7 +2578,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="35" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B3" s="36"/>
       <c r="C3" s="36"/>
@@ -2616,7 +2616,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="34" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B7" s="34"/>
       <c r="C7" s="34"/>
@@ -2654,7 +2654,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="35" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B9" s="36"/>
       <c r="C9" s="36"/>
@@ -2692,7 +2692,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="34" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B13" s="34"/>
       <c r="C13" s="34"/>
@@ -2730,7 +2730,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="35" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B15" s="36"/>
       <c r="C15" s="36"/>
@@ -2768,7 +2768,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="34" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B19" s="34"/>
       <c r="C19" s="34"/>
@@ -2806,7 +2806,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="35" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B21" s="36"/>
       <c r="C21" s="36"/>
@@ -2844,7 +2844,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="34" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B25" s="34"/>
       <c r="C25" s="34"/>
@@ -2934,7 +2934,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="34" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B31" s="34"/>
       <c r="C31" s="34"/>
@@ -3018,7 +3018,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="34" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B37" s="34"/>
       <c r="C37" s="34"/>
@@ -3062,22 +3062,22 @@
         <v>0</v>
       </c>
       <c r="C39" s="21" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D39" s="21" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F39" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="H39" s="21" t="s">
         <v>93</v>
-      </c>
-      <c r="G39" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="H39" s="21" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Fixed SYS3 Bitorder inconsistency
</commit_message>
<xml_diff>
--- a/Doc/Encodings.xlsx
+++ b/Doc/Encodings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pschilk\home\Repos\psMCU\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A8744D-B280-463B-A1F7-D050BD1150FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{999230C6-BBF1-447C-96B2-CF573C002776}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35955" yWindow="1530" windowWidth="17040" windowHeight="12480" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inst Decoding" sheetId="2" r:id="rId1"/>
@@ -311,9 +311,6 @@
     <t>A&gt;B</t>
   </si>
   <si>
-    <t>B&lt;A</t>
-  </si>
-  <si>
     <t>Scratch Reg 1 (Adr 0x100)</t>
   </si>
   <si>
@@ -432,6 +429,9 @@
   </si>
   <si>
     <t>SUB(L)</t>
+  </si>
+  <si>
+    <t>A&lt;B</t>
   </si>
 </sst>
 </file>
@@ -2312,7 +2312,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59778E2C-D2B8-41E1-8336-5F65E1F1812B}">
   <dimension ref="A1:R667"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
@@ -2371,37 +2371,37 @@
     </row>
     <row r="2" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="38" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="H2" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="I2" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="J2" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="B2" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="C2" s="30" t="s">
-        <v>128</v>
-      </c>
-      <c r="D2" s="30" t="s">
-        <v>128</v>
-      </c>
-      <c r="E2" s="30" t="s">
-        <v>128</v>
-      </c>
-      <c r="F2" s="30" t="s">
-        <v>128</v>
-      </c>
-      <c r="G2" s="30" t="s">
-        <v>128</v>
-      </c>
-      <c r="H2" s="30" t="s">
-        <v>128</v>
-      </c>
-      <c r="I2" s="30" t="s">
-        <v>128</v>
-      </c>
-      <c r="J2" s="13" t="s">
+      <c r="K2" s="13" t="s">
         <v>130</v>
-      </c>
-      <c r="K2" s="13" t="s">
-        <v>131</v>
       </c>
       <c r="L2" s="13">
         <v>128</v>
@@ -2437,7 +2437,7 @@
         <v>51</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L3" s="13">
         <v>32</v>
@@ -2473,7 +2473,7 @@
         <v>50</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L4" s="13">
         <v>32</v>
@@ -2490,7 +2490,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C5" s="8">
         <v>0</v>
@@ -2502,7 +2502,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G5" s="43" t="s">
         <v>11</v>
@@ -2513,7 +2513,7 @@
         <v>49</v>
       </c>
       <c r="K5" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L5" s="13">
         <v>16</v>
@@ -2530,7 +2530,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C6" s="8">
         <v>0</v>
@@ -2542,7 +2542,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G6" s="43" t="s">
         <v>11</v>
@@ -2553,7 +2553,7 @@
         <v>48</v>
       </c>
       <c r="K6" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L6" s="13">
         <v>16</v>
@@ -2567,10 +2567,10 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="36" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C7" s="8">
         <v>0</v>
@@ -2594,7 +2594,7 @@
         <v>1</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K7" s="13" t="s">
         <v>29</v>
@@ -2611,10 +2611,10 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="36" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C8" s="8">
         <v>0</v>
@@ -2638,7 +2638,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K8" s="13" t="s">
         <v>29</v>
@@ -2655,10 +2655,10 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="37" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C9" s="8">
         <v>0</v>
@@ -2682,10 +2682,10 @@
         <v>1</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K9" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L9" s="13">
         <v>1</v>
@@ -2699,10 +2699,10 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C10" s="8">
         <v>0</v>
@@ -2726,7 +2726,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K10" s="13" t="s">
         <v>92</v>
@@ -2743,10 +2743,10 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C11" s="8">
         <v>0</v>
@@ -2770,7 +2770,7 @@
         <v>1</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K11" s="13" t="s">
         <v>61</v>
@@ -2787,10 +2787,10 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="37" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C12" s="8">
         <v>0</v>
@@ -2814,7 +2814,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K12" s="13" t="s">
         <v>60</v>
@@ -2831,10 +2831,10 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="37" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C13" s="8">
         <v>0</v>
@@ -2858,7 +2858,7 @@
         <v>1</v>
       </c>
       <c r="J13" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K13" s="13" t="s">
         <v>59</v>
@@ -3140,7 +3140,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C20" s="8">
         <v>0</v>
@@ -3184,7 +3184,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C21" s="8">
         <v>0</v>
@@ -3228,7 +3228,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C22" s="8">
         <v>0</v>
@@ -3401,10 +3401,10 @@
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="B26" s="19" t="s">
         <v>133</v>
-      </c>
-      <c r="B26" s="19" t="s">
-        <v>134</v>
       </c>
       <c r="C26" s="8">
         <v>0</v>
@@ -3489,10 +3489,10 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C28" s="8">
         <v>0</v>
@@ -3533,10 +3533,10 @@
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C29" s="8">
         <v>0</v>
@@ -6406,8 +6406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D74D41B-283E-4F55-BA94-91EF2EF7E1E9}">
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6419,7 +6419,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1" s="46"/>
       <c r="C1" s="46"/>
@@ -6457,7 +6457,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B3" s="48"/>
       <c r="C3" s="48"/>
@@ -6495,7 +6495,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="46" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B7" s="46"/>
       <c r="C7" s="46"/>
@@ -6533,7 +6533,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="47" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B9" s="48"/>
       <c r="C9" s="48"/>
@@ -6571,7 +6571,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="46" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B13" s="46"/>
       <c r="C13" s="46"/>
@@ -6609,7 +6609,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="47" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B15" s="48"/>
       <c r="C15" s="48"/>
@@ -6647,7 +6647,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="46" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B19" s="46"/>
       <c r="C19" s="46"/>
@@ -6685,7 +6685,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="47" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B21" s="48"/>
       <c r="C21" s="48"/>
@@ -6723,7 +6723,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="46" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B25" s="46"/>
       <c r="C25" s="46"/>
@@ -6813,7 +6813,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B31" s="46"/>
       <c r="C31" s="46"/>
@@ -6897,7 +6897,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="46" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B37" s="46"/>
       <c r="C37" s="46"/>
@@ -6941,10 +6941,10 @@
         <v>0</v>
       </c>
       <c r="C39" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="D39" s="20" t="s">
         <v>93</v>
-      </c>
-      <c r="D39" s="20" t="s">
-        <v>94</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>85</v>

</xml_diff>

<commit_message>
First Schematic Draft done.
</commit_message>
<xml_diff>
--- a/Doc/Encodings.xlsx
+++ b/Doc/Encodings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pschilk\home\Repos\psMCU\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{999230C6-BBF1-447C-96B2-CF573C002776}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D303F92-7564-4DDD-A880-7E379E713497}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35955" yWindow="1530" windowWidth="17040" windowHeight="12480" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inst Decoding" sheetId="2" r:id="rId1"/>
@@ -41,9 +41,6 @@
     <t>OR</t>
   </si>
   <si>
-    <t>NOR</t>
-  </si>
-  <si>
     <t>Unused</t>
   </si>
   <si>
@@ -432,6 +429,9 @@
   </si>
   <si>
     <t>A&lt;B</t>
+  </si>
+  <si>
+    <t>XOR</t>
   </si>
 </sst>
 </file>
@@ -2316,21 +2316,21 @@
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" customWidth="1"/>
-    <col min="2" max="2" width="16.77734375" style="19" customWidth="1"/>
-    <col min="10" max="10" width="11.109375" style="15" customWidth="1"/>
-    <col min="11" max="11" width="13.88671875" style="15" customWidth="1"/>
-    <col min="12" max="18" width="8.88671875" style="15"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" style="19" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" style="15" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" style="15" customWidth="1"/>
+    <col min="12" max="18" width="8.85546875" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C1" s="2">
         <v>15</v>
@@ -2354,13 +2354,13 @@
         <v>9</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L1" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M1" s="13"/>
       <c r="N1" s="13"/>
@@ -2369,39 +2369,39 @@
       <c r="Q1" s="13"/>
       <c r="R1" s="13"/>
     </row>
-    <row r="2" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="38" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="H2" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="I2" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="J2" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="B2" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="C2" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="D2" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="E2" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="F2" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="G2" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="H2" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="I2" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="J2" s="13" t="s">
+      <c r="K2" s="13" t="s">
         <v>129</v>
-      </c>
-      <c r="K2" s="13" t="s">
-        <v>130</v>
       </c>
       <c r="L2" s="13">
         <v>128</v>
@@ -2413,31 +2413,31 @@
       <c r="Q2" s="13"/>
       <c r="R2" s="13"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1</v>
+      </c>
+      <c r="D3" s="6">
+        <v>1</v>
+      </c>
+      <c r="E3" s="39" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="C3" s="5">
-        <v>1</v>
-      </c>
-      <c r="D3" s="6">
-        <v>1</v>
-      </c>
-      <c r="E3" s="39" t="s">
-        <v>8</v>
       </c>
       <c r="F3" s="40"/>
       <c r="G3" s="40"/>
       <c r="H3" s="40"/>
       <c r="I3" s="40"/>
       <c r="J3" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L3" s="13">
         <v>32</v>
@@ -2449,12 +2449,12 @@
       <c r="Q3" s="14"/>
       <c r="R3" s="14"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C4" s="8">
         <v>1</v>
@@ -2463,17 +2463,17 @@
         <v>0</v>
       </c>
       <c r="E4" s="41" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4" s="42"/>
       <c r="G4" s="42"/>
       <c r="H4" s="42"/>
       <c r="I4" s="42"/>
       <c r="J4" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L4" s="13">
         <v>32</v>
@@ -2485,35 +2485,35 @@
       <c r="Q4" s="14"/>
       <c r="R4" s="14"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="8">
+        <v>0</v>
+      </c>
+      <c r="D5" s="6">
+        <v>1</v>
+      </c>
+      <c r="E5" s="6">
+        <v>1</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="G5" s="43" t="s">
         <v>10</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="C5" s="8">
-        <v>0</v>
-      </c>
-      <c r="D5" s="6">
-        <v>1</v>
-      </c>
-      <c r="E5" s="6">
-        <v>1</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="G5" s="43" t="s">
-        <v>11</v>
       </c>
       <c r="H5" s="43"/>
       <c r="I5" s="43"/>
       <c r="J5" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K5" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L5" s="13">
         <v>16</v>
@@ -2525,12 +2525,12 @@
       <c r="Q5" s="13"/>
       <c r="R5" s="13"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="35" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C6" s="8">
         <v>0</v>
@@ -2542,18 +2542,18 @@
         <v>0</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G6" s="43" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H6" s="43"/>
       <c r="I6" s="43"/>
       <c r="J6" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K6" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L6" s="13">
         <v>16</v>
@@ -2565,12 +2565,12 @@
       <c r="Q6" s="13"/>
       <c r="R6" s="13"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="36" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C7" s="8">
         <v>0</v>
@@ -2594,10 +2594,10 @@
         <v>1</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K7" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L7" s="13">
         <v>1</v>
@@ -2609,12 +2609,12 @@
       <c r="Q7" s="13"/>
       <c r="R7" s="13"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C8" s="8">
         <v>0</v>
@@ -2638,10 +2638,10 @@
         <v>0</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K8" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L8" s="13">
         <v>1</v>
@@ -2653,12 +2653,12 @@
       <c r="Q8" s="13"/>
       <c r="R8" s="13"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="37" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C9" s="8">
         <v>0</v>
@@ -2682,10 +2682,10 @@
         <v>1</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K9" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L9" s="13">
         <v>1</v>
@@ -2697,12 +2697,12 @@
       <c r="Q9" s="13"/>
       <c r="R9" s="13"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="37" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C10" s="8">
         <v>0</v>
@@ -2726,10 +2726,10 @@
         <v>0</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K10" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L10" s="13">
         <v>1</v>
@@ -2741,12 +2741,12 @@
       <c r="Q10" s="13"/>
       <c r="R10" s="13"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C11" s="8">
         <v>0</v>
@@ -2770,10 +2770,10 @@
         <v>1</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K11" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L11" s="13">
         <v>1</v>
@@ -2785,12 +2785,12 @@
       <c r="Q11" s="13"/>
       <c r="R11" s="13"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C12" s="8">
         <v>0</v>
@@ -2814,10 +2814,10 @@
         <v>0</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K12" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L12" s="13">
         <v>1</v>
@@ -2829,12 +2829,12 @@
       <c r="Q12" s="13"/>
       <c r="R12" s="13"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="37" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C13" s="8">
         <v>0</v>
@@ -2858,10 +2858,10 @@
         <v>1</v>
       </c>
       <c r="J13" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K13" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L13" s="13">
         <v>1</v>
@@ -2873,39 +2873,39 @@
       <c r="Q13" s="13"/>
       <c r="R13" s="13"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0</v>
+      </c>
+      <c r="D14" s="22">
+        <v>0</v>
+      </c>
+      <c r="E14" s="23">
+        <v>1</v>
+      </c>
+      <c r="F14" s="9">
+        <v>1</v>
+      </c>
+      <c r="G14" s="21">
+        <v>0</v>
+      </c>
+      <c r="H14" s="21">
+        <v>0</v>
+      </c>
+      <c r="I14" s="21">
+        <v>0</v>
+      </c>
+      <c r="J14" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="B14" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="C14" s="8">
-        <v>0</v>
-      </c>
-      <c r="D14" s="22">
-        <v>0</v>
-      </c>
-      <c r="E14" s="23">
-        <v>1</v>
-      </c>
-      <c r="F14" s="9">
-        <v>1</v>
-      </c>
-      <c r="G14" s="21">
-        <v>0</v>
-      </c>
-      <c r="H14" s="21">
-        <v>0</v>
-      </c>
-      <c r="I14" s="21">
-        <v>0</v>
-      </c>
-      <c r="J14" s="13" t="s">
-        <v>91</v>
-      </c>
       <c r="K14" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L14" s="13">
         <v>1</v>
@@ -2917,37 +2917,37 @@
       <c r="Q14" s="13"/>
       <c r="R14" s="13"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="8">
+        <v>0</v>
+      </c>
+      <c r="D15" s="6">
+        <v>0</v>
+      </c>
+      <c r="E15" s="6">
+        <v>1</v>
+      </c>
+      <c r="F15" s="6">
+        <v>0</v>
+      </c>
+      <c r="G15" s="6">
+        <v>1</v>
+      </c>
+      <c r="H15" s="44" t="s">
         <v>13</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="C15" s="8">
-        <v>0</v>
-      </c>
-      <c r="D15" s="6">
-        <v>0</v>
-      </c>
-      <c r="E15" s="6">
-        <v>1</v>
-      </c>
-      <c r="F15" s="6">
-        <v>0</v>
-      </c>
-      <c r="G15" s="6">
-        <v>1</v>
-      </c>
-      <c r="H15" s="44" t="s">
-        <v>14</v>
       </c>
       <c r="I15" s="44"/>
       <c r="J15" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K15" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L15" s="13">
         <v>4</v>
@@ -2959,39 +2959,39 @@
       <c r="Q15" s="13"/>
       <c r="R15" s="13"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="8">
+        <v>0</v>
+      </c>
+      <c r="D16" s="6">
+        <v>0</v>
+      </c>
+      <c r="E16" s="6">
+        <v>1</v>
+      </c>
+      <c r="F16" s="6">
+        <v>0</v>
+      </c>
+      <c r="G16" s="6">
+        <v>0</v>
+      </c>
+      <c r="H16" s="6">
+        <v>1</v>
+      </c>
+      <c r="I16" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="C16" s="8">
-        <v>0</v>
-      </c>
-      <c r="D16" s="6">
-        <v>0</v>
-      </c>
-      <c r="E16" s="6">
-        <v>1</v>
-      </c>
-      <c r="F16" s="6">
-        <v>0</v>
-      </c>
-      <c r="G16" s="6">
-        <v>0</v>
-      </c>
-      <c r="H16" s="6">
-        <v>1</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>17</v>
-      </c>
       <c r="J16" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K16" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L16" s="13">
         <v>2</v>
@@ -3003,12 +3003,12 @@
       <c r="Q16" s="13"/>
       <c r="R16" s="13"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C17" s="8">
         <v>0</v>
@@ -3029,13 +3029,13 @@
         <v>0</v>
       </c>
       <c r="I17" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K17" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L17" s="13">
         <v>2</v>
@@ -3047,12 +3047,12 @@
       <c r="Q17" s="13"/>
       <c r="R17" s="13"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C18" s="8">
         <v>0</v>
@@ -3073,13 +3073,13 @@
         <v>1</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J18" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K18" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L18" s="13">
         <v>2</v>
@@ -3091,12 +3091,12 @@
       <c r="Q18" s="13"/>
       <c r="R18" s="13"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C19" s="8">
         <v>0</v>
@@ -3120,10 +3120,10 @@
         <v>1</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K19" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L19" s="13">
         <v>1</v>
@@ -3135,12 +3135,12 @@
       <c r="Q19" s="13"/>
       <c r="R19" s="13"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C20" s="8">
         <v>0</v>
@@ -3164,10 +3164,10 @@
         <v>0</v>
       </c>
       <c r="J20" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K20" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L20" s="13">
         <v>1</v>
@@ -3179,12 +3179,12 @@
       <c r="Q20" s="13"/>
       <c r="R20" s="13"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C21" s="8">
         <v>0</v>
@@ -3208,10 +3208,10 @@
         <v>1</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K21" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L21" s="13">
         <v>1</v>
@@ -3223,12 +3223,12 @@
       <c r="Q21" s="13"/>
       <c r="R21" s="13"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C22" s="8">
         <v>0</v>
@@ -3252,10 +3252,10 @@
         <v>0</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K22" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L22" s="13">
         <v>1</v>
@@ -3267,12 +3267,12 @@
       <c r="Q22" s="13"/>
       <c r="R22" s="13"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C23" s="8">
         <v>0</v>
@@ -3296,10 +3296,10 @@
         <v>1</v>
       </c>
       <c r="J23" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K23" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L23" s="13">
         <v>1</v>
@@ -3311,12 +3311,12 @@
       <c r="Q23" s="13"/>
       <c r="R23" s="13"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C24" s="8">
         <v>0</v>
@@ -3340,10 +3340,10 @@
         <v>0</v>
       </c>
       <c r="J24" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K24" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L24" s="13">
         <v>1</v>
@@ -3355,13 +3355,13 @@
       <c r="Q24" s="13"/>
       <c r="R24" s="13"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="B25" s="19" t="s">
-        <v>87</v>
-      </c>
       <c r="C25" s="8">
         <v>0</v>
       </c>
@@ -3384,10 +3384,10 @@
         <v>1</v>
       </c>
       <c r="J25" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K25" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L25" s="13">
         <v>1</v>
@@ -3399,13 +3399,13 @@
       <c r="Q25" s="13"/>
       <c r="R25" s="13"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B26" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="B26" s="19" t="s">
-        <v>133</v>
-      </c>
       <c r="C26" s="8">
         <v>0</v>
       </c>
@@ -3428,10 +3428,10 @@
         <v>0</v>
       </c>
       <c r="J26" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K26" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L26" s="13">
         <v>1</v>
@@ -3443,12 +3443,12 @@
       <c r="Q26" s="13"/>
       <c r="R26" s="13"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C27" s="8">
         <v>0</v>
@@ -3472,10 +3472,10 @@
         <v>1</v>
       </c>
       <c r="J27" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K27" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L27" s="13">
         <v>1</v>
@@ -3487,12 +3487,12 @@
       <c r="Q27" s="13"/>
       <c r="R27" s="13"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C28" s="8">
         <v>0</v>
@@ -3516,10 +3516,10 @@
         <v>0</v>
       </c>
       <c r="J28" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K28" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L28" s="13">
         <v>1</v>
@@ -3531,12 +3531,12 @@
       <c r="Q28" s="13"/>
       <c r="R28" s="13"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C29" s="8">
         <v>0</v>
@@ -3560,10 +3560,10 @@
         <v>1</v>
       </c>
       <c r="J29" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K29" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L29" s="13">
         <v>1</v>
@@ -3575,12 +3575,12 @@
       <c r="Q29" s="13"/>
       <c r="R29" s="13"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C30" s="8">
         <v>0</v>
@@ -3604,10 +3604,10 @@
         <v>0</v>
       </c>
       <c r="J30" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K30" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L30" s="13">
         <v>1</v>
@@ -3619,12 +3619,12 @@
       <c r="Q30" s="13"/>
       <c r="R30" s="13"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C31" s="8">
         <v>0</v>
@@ -3648,10 +3648,10 @@
         <v>1</v>
       </c>
       <c r="J31" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K31" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L31" s="13">
         <v>1</v>
@@ -3663,12 +3663,12 @@
       <c r="Q31" s="13"/>
       <c r="R31" s="13"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C32" s="8">
         <v>0</v>
@@ -3692,10 +3692,10 @@
         <v>0</v>
       </c>
       <c r="J32" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K32" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L32" s="13">
         <v>1</v>
@@ -3707,1909 +3707,1909 @@
       <c r="Q32" s="13"/>
       <c r="R32" s="13"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="32"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="33"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="33"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="33"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" s="33"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" s="33"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" s="33"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" s="33"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" s="33"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" s="33"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" s="33"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" s="33"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" s="33"/>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46" s="33"/>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" s="33"/>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" s="33"/>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" s="33"/>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" s="33"/>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" s="33"/>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" s="33"/>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53" s="33"/>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" s="33"/>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55" s="33"/>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" s="33"/>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B57" s="33"/>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B58" s="33"/>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" s="33"/>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" s="33"/>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" s="33"/>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B62" s="33"/>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B63" s="33"/>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B64" s="33"/>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" s="33"/>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" s="33"/>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" s="33"/>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" s="33"/>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69" s="33"/>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70" s="33"/>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" s="33"/>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72" s="33"/>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B73" s="33"/>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B74" s="33"/>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B75" s="33"/>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B76" s="33"/>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B77" s="33"/>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B78" s="33"/>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B79" s="33"/>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B80" s="33"/>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" s="33"/>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B82" s="33"/>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83" s="33"/>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84" s="33"/>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85" s="33"/>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B86" s="33"/>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B87" s="33"/>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B88" s="33"/>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B89" s="33"/>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B90" s="33"/>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B91" s="33"/>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B92" s="33"/>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B93" s="33"/>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B94" s="33"/>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B95" s="33"/>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B96" s="33"/>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B97" s="33"/>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B98" s="33"/>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B99" s="33"/>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B100" s="33"/>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B101" s="33"/>
     </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B102" s="33"/>
     </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B103" s="33"/>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B104" s="33"/>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B105" s="33"/>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B106" s="33"/>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B107" s="33"/>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B108" s="33"/>
     </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B109" s="33"/>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B110" s="33"/>
     </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B111" s="33"/>
     </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B112" s="33"/>
     </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B113" s="33"/>
     </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B114" s="33"/>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B115" s="33"/>
     </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B116" s="33"/>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B117" s="33"/>
     </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B118" s="33"/>
     </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B119" s="33"/>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B120" s="33"/>
     </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B121" s="33"/>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B122" s="33"/>
     </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B123" s="33"/>
     </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B124" s="33"/>
     </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B125" s="33"/>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B126" s="33"/>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B127" s="33"/>
     </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B128" s="33"/>
     </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B129" s="33"/>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B130" s="33"/>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B131" s="33"/>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B132" s="33"/>
     </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B133" s="33"/>
     </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B134" s="33"/>
     </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B135" s="33"/>
     </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B136" s="33"/>
     </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B137" s="33"/>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B138" s="33"/>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B139" s="33"/>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B140" s="33"/>
     </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B141" s="33"/>
     </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B142" s="33"/>
     </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B143" s="33"/>
     </row>
-    <row r="144" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B144" s="33"/>
     </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B145" s="33"/>
     </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B146" s="33"/>
     </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B147" s="33"/>
     </row>
-    <row r="148" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B148" s="33"/>
     </row>
-    <row r="149" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B149" s="33"/>
     </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B150" s="33"/>
     </row>
-    <row r="151" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B151" s="33"/>
     </row>
-    <row r="152" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B152" s="33"/>
     </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B153" s="33"/>
     </row>
-    <row r="154" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B154" s="33"/>
     </row>
-    <row r="155" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B155" s="33"/>
     </row>
-    <row r="156" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B156" s="33"/>
     </row>
-    <row r="157" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="157" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B157" s="33"/>
     </row>
-    <row r="158" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="158" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B158" s="33"/>
     </row>
-    <row r="159" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="159" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B159" s="33"/>
     </row>
-    <row r="160" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="160" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B160" s="33"/>
     </row>
-    <row r="161" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="161" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B161" s="33"/>
     </row>
-    <row r="162" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="162" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B162" s="33"/>
     </row>
-    <row r="163" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="163" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B163" s="33"/>
     </row>
-    <row r="164" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="164" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B164" s="33"/>
     </row>
-    <row r="165" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="165" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B165" s="33"/>
     </row>
-    <row r="166" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="166" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B166" s="33"/>
     </row>
-    <row r="167" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="167" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B167" s="33"/>
     </row>
-    <row r="168" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="168" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B168" s="33"/>
     </row>
-    <row r="169" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="169" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B169" s="33"/>
     </row>
-    <row r="170" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="170" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B170" s="33"/>
     </row>
-    <row r="171" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="171" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B171" s="33"/>
     </row>
-    <row r="172" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="172" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B172" s="33"/>
     </row>
-    <row r="173" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="173" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B173" s="33"/>
     </row>
-    <row r="174" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="174" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B174" s="33"/>
     </row>
-    <row r="175" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="175" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B175" s="33"/>
     </row>
-    <row r="176" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="176" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B176" s="33"/>
     </row>
-    <row r="177" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="177" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B177" s="33"/>
     </row>
-    <row r="178" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="178" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B178" s="33"/>
     </row>
-    <row r="179" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="179" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B179" s="33"/>
     </row>
-    <row r="180" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="180" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B180" s="33"/>
     </row>
-    <row r="181" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="181" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B181" s="33"/>
     </row>
-    <row r="182" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="182" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B182" s="33"/>
     </row>
-    <row r="183" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="183" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B183" s="33"/>
     </row>
-    <row r="184" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="184" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B184" s="33"/>
     </row>
-    <row r="185" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="185" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B185" s="33"/>
     </row>
-    <row r="186" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="186" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B186" s="33"/>
     </row>
-    <row r="187" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="187" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B187" s="33"/>
     </row>
-    <row r="188" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="188" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B188" s="33"/>
     </row>
-    <row r="189" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="189" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B189" s="33"/>
     </row>
-    <row r="190" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="190" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B190" s="33"/>
     </row>
-    <row r="191" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="191" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B191" s="33"/>
     </row>
-    <row r="192" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="192" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B192" s="33"/>
     </row>
-    <row r="193" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="193" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B193" s="33"/>
     </row>
-    <row r="194" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="194" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B194" s="33"/>
     </row>
-    <row r="195" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="195" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B195" s="33"/>
     </row>
-    <row r="196" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="196" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B196" s="33"/>
     </row>
-    <row r="197" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="197" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B197" s="33"/>
     </row>
-    <row r="198" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="198" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B198" s="33"/>
     </row>
-    <row r="199" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="199" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B199" s="33"/>
     </row>
-    <row r="200" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="200" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B200" s="33"/>
     </row>
-    <row r="201" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="201" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B201" s="33"/>
     </row>
-    <row r="202" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="202" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B202" s="33"/>
     </row>
-    <row r="203" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="203" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B203" s="33"/>
     </row>
-    <row r="204" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="204" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B204" s="33"/>
     </row>
-    <row r="205" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="205" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B205" s="33"/>
     </row>
-    <row r="206" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="206" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B206" s="33"/>
     </row>
-    <row r="207" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="207" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B207" s="33"/>
     </row>
-    <row r="208" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="208" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B208" s="33"/>
     </row>
-    <row r="209" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="209" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B209" s="33"/>
     </row>
-    <row r="210" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="210" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B210" s="33"/>
     </row>
-    <row r="211" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="211" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B211" s="33"/>
     </row>
-    <row r="212" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="212" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B212" s="33"/>
     </row>
-    <row r="213" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="213" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B213" s="33"/>
     </row>
-    <row r="214" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="214" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B214" s="33"/>
     </row>
-    <row r="215" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="215" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B215" s="33"/>
     </row>
-    <row r="216" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="216" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B216" s="33"/>
     </row>
-    <row r="217" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="217" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B217" s="33"/>
     </row>
-    <row r="218" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="218" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B218" s="33"/>
     </row>
-    <row r="219" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="219" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B219" s="33"/>
     </row>
-    <row r="220" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="220" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B220" s="33"/>
     </row>
-    <row r="221" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="221" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B221" s="33"/>
     </row>
-    <row r="222" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="222" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B222" s="33"/>
     </row>
-    <row r="223" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="223" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B223" s="33"/>
     </row>
-    <row r="224" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="224" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B224" s="33"/>
     </row>
-    <row r="225" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="225" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B225" s="33"/>
     </row>
-    <row r="226" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="226" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B226" s="33"/>
     </row>
-    <row r="227" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="227" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B227" s="33"/>
     </row>
-    <row r="228" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="228" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B228" s="33"/>
     </row>
-    <row r="229" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="229" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B229" s="33"/>
     </row>
-    <row r="230" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="230" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B230" s="33"/>
     </row>
-    <row r="231" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="231" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B231" s="33"/>
     </row>
-    <row r="232" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="232" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B232" s="33"/>
     </row>
-    <row r="233" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="233" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B233" s="33"/>
     </row>
-    <row r="234" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="234" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B234" s="33"/>
     </row>
-    <row r="235" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="235" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B235" s="33"/>
     </row>
-    <row r="236" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="236" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B236" s="33"/>
     </row>
-    <row r="237" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="237" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B237" s="33"/>
     </row>
-    <row r="238" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="238" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B238" s="33"/>
     </row>
-    <row r="239" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="239" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B239" s="33"/>
     </row>
-    <row r="240" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="240" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B240" s="33"/>
     </row>
-    <row r="241" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="241" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B241" s="33"/>
     </row>
-    <row r="242" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="242" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B242" s="33"/>
     </row>
-    <row r="243" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="243" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B243" s="33"/>
     </row>
-    <row r="244" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="244" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B244" s="33"/>
     </row>
-    <row r="245" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="245" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B245" s="33"/>
     </row>
-    <row r="246" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="246" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B246" s="33"/>
     </row>
-    <row r="247" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="247" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B247" s="33"/>
     </row>
-    <row r="248" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="248" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B248" s="33"/>
     </row>
-    <row r="249" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="249" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B249" s="33"/>
     </row>
-    <row r="250" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="250" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B250" s="33"/>
     </row>
-    <row r="251" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="251" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B251" s="33"/>
     </row>
-    <row r="252" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="252" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B252" s="33"/>
     </row>
-    <row r="253" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="253" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B253" s="33"/>
     </row>
-    <row r="254" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="254" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B254" s="33"/>
     </row>
-    <row r="255" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="255" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B255" s="33"/>
     </row>
-    <row r="256" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="256" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B256" s="33"/>
     </row>
-    <row r="257" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="257" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B257" s="33"/>
     </row>
-    <row r="258" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="258" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B258" s="33"/>
     </row>
-    <row r="259" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="259" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B259" s="33"/>
     </row>
-    <row r="260" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="260" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B260" s="33"/>
     </row>
-    <row r="261" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="261" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B261" s="33"/>
     </row>
-    <row r="262" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="262" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B262" s="33"/>
     </row>
-    <row r="263" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="263" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B263" s="33"/>
     </row>
-    <row r="264" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="264" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B264" s="33"/>
     </row>
-    <row r="265" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="265" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B265" s="33"/>
     </row>
-    <row r="266" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="266" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B266" s="33"/>
     </row>
-    <row r="267" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="267" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B267" s="33"/>
     </row>
-    <row r="268" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="268" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B268" s="33"/>
     </row>
-    <row r="269" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="269" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B269" s="33"/>
     </row>
-    <row r="270" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="270" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B270" s="33"/>
     </row>
-    <row r="271" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="271" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B271" s="33"/>
     </row>
-    <row r="272" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="272" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B272" s="33"/>
     </row>
-    <row r="273" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="273" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B273" s="33"/>
     </row>
-    <row r="274" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="274" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B274" s="33"/>
     </row>
-    <row r="275" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="275" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B275" s="33"/>
     </row>
-    <row r="276" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="276" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B276" s="33"/>
     </row>
-    <row r="277" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="277" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B277" s="33"/>
     </row>
-    <row r="278" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="278" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B278" s="33"/>
     </row>
-    <row r="279" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="279" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B279" s="33"/>
     </row>
-    <row r="280" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="280" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B280" s="33"/>
     </row>
-    <row r="281" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="281" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B281" s="33"/>
     </row>
-    <row r="282" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="282" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B282" s="33"/>
     </row>
-    <row r="283" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="283" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B283" s="33"/>
     </row>
-    <row r="284" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="284" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B284" s="33"/>
     </row>
-    <row r="285" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="285" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B285" s="33"/>
     </row>
-    <row r="286" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="286" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B286" s="33"/>
     </row>
-    <row r="287" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="287" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B287" s="33"/>
     </row>
-    <row r="288" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="288" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B288" s="33"/>
     </row>
-    <row r="289" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="289" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B289" s="33"/>
     </row>
-    <row r="290" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="290" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B290" s="33"/>
     </row>
-    <row r="291" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="291" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B291" s="33"/>
     </row>
-    <row r="292" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="292" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B292" s="33"/>
     </row>
-    <row r="293" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="293" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B293" s="33"/>
     </row>
-    <row r="294" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="294" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B294" s="33"/>
     </row>
-    <row r="295" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="295" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B295" s="33"/>
     </row>
-    <row r="296" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="296" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B296" s="33"/>
     </row>
-    <row r="297" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="297" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B297" s="33"/>
     </row>
-    <row r="298" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="298" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B298" s="33"/>
     </row>
-    <row r="299" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="299" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B299" s="33"/>
     </row>
-    <row r="300" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="300" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B300" s="33"/>
     </row>
-    <row r="301" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="301" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B301" s="33"/>
     </row>
-    <row r="302" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="302" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B302" s="33"/>
     </row>
-    <row r="303" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="303" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B303" s="33"/>
     </row>
-    <row r="304" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="304" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B304" s="33"/>
     </row>
-    <row r="305" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="305" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B305" s="33"/>
     </row>
-    <row r="306" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="306" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B306" s="33"/>
     </row>
-    <row r="307" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="307" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B307" s="33"/>
     </row>
-    <row r="308" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="308" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B308" s="33"/>
     </row>
-    <row r="309" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="309" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B309" s="33"/>
     </row>
-    <row r="310" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="310" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B310" s="33"/>
     </row>
-    <row r="311" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="311" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B311" s="33"/>
     </row>
-    <row r="312" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="312" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B312" s="33"/>
     </row>
-    <row r="313" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="313" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B313" s="33"/>
     </row>
-    <row r="314" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="314" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B314" s="33"/>
     </row>
-    <row r="315" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="315" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B315" s="33"/>
     </row>
-    <row r="316" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="316" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B316" s="33"/>
     </row>
-    <row r="317" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="317" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B317" s="33"/>
     </row>
-    <row r="318" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="318" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B318" s="33"/>
     </row>
-    <row r="319" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="319" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B319" s="33"/>
     </row>
-    <row r="320" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="320" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B320" s="33"/>
     </row>
-    <row r="321" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="321" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B321" s="33"/>
     </row>
-    <row r="322" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="322" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B322" s="33"/>
     </row>
-    <row r="323" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="323" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B323" s="33"/>
     </row>
-    <row r="324" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="324" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B324" s="33"/>
     </row>
-    <row r="325" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="325" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B325" s="33"/>
     </row>
-    <row r="326" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="326" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B326" s="33"/>
     </row>
-    <row r="327" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="327" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B327" s="33"/>
     </row>
-    <row r="328" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="328" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B328" s="33"/>
     </row>
-    <row r="329" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="329" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B329" s="33"/>
     </row>
-    <row r="330" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="330" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B330" s="33"/>
     </row>
-    <row r="331" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="331" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B331" s="33"/>
     </row>
-    <row r="332" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="332" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B332" s="33"/>
     </row>
-    <row r="333" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="333" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B333" s="33"/>
     </row>
-    <row r="334" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="334" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B334" s="33"/>
     </row>
-    <row r="335" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="335" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B335" s="33"/>
     </row>
-    <row r="336" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="336" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B336" s="33"/>
     </row>
-    <row r="337" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="337" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B337" s="33"/>
     </row>
-    <row r="338" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="338" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B338" s="33"/>
     </row>
-    <row r="339" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="339" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B339" s="33"/>
     </row>
-    <row r="340" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="340" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B340" s="33"/>
     </row>
-    <row r="341" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="341" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B341" s="33"/>
     </row>
-    <row r="342" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="342" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B342" s="33"/>
     </row>
-    <row r="343" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="343" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B343" s="33"/>
     </row>
-    <row r="344" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="344" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B344" s="33"/>
     </row>
-    <row r="345" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="345" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B345" s="33"/>
     </row>
-    <row r="346" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="346" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B346" s="33"/>
     </row>
-    <row r="347" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="347" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B347" s="33"/>
     </row>
-    <row r="348" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="348" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B348" s="33"/>
     </row>
-    <row r="349" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="349" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B349" s="33"/>
     </row>
-    <row r="350" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="350" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B350" s="33"/>
     </row>
-    <row r="351" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="351" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B351" s="33"/>
     </row>
-    <row r="352" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="352" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B352" s="33"/>
     </row>
-    <row r="353" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="353" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B353" s="33"/>
     </row>
-    <row r="354" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="354" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B354" s="33"/>
     </row>
-    <row r="355" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="355" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B355" s="33"/>
     </row>
-    <row r="356" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="356" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B356" s="33"/>
     </row>
-    <row r="357" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="357" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B357" s="33"/>
     </row>
-    <row r="358" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="358" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B358" s="33"/>
     </row>
-    <row r="359" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="359" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B359" s="33"/>
     </row>
-    <row r="360" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="360" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B360" s="33"/>
     </row>
-    <row r="361" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="361" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B361" s="33"/>
     </row>
-    <row r="362" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="362" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B362" s="33"/>
     </row>
-    <row r="363" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="363" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B363" s="33"/>
     </row>
-    <row r="364" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="364" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B364" s="33"/>
     </row>
-    <row r="365" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="365" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B365" s="33"/>
     </row>
-    <row r="366" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="366" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B366" s="33"/>
     </row>
-    <row r="367" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="367" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B367" s="33"/>
     </row>
-    <row r="368" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="368" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B368" s="33"/>
     </row>
-    <row r="369" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="369" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B369" s="33"/>
     </row>
-    <row r="370" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="370" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B370" s="33"/>
     </row>
-    <row r="371" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="371" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B371" s="33"/>
     </row>
-    <row r="372" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="372" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B372" s="33"/>
     </row>
-    <row r="373" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="373" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B373" s="33"/>
     </row>
-    <row r="374" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="374" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B374" s="33"/>
     </row>
-    <row r="375" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="375" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B375" s="33"/>
     </row>
-    <row r="376" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="376" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B376" s="33"/>
     </row>
-    <row r="377" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="377" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B377" s="33"/>
     </row>
-    <row r="378" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="378" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B378" s="33"/>
     </row>
-    <row r="379" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="379" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B379" s="33"/>
     </row>
-    <row r="380" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="380" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B380" s="33"/>
     </row>
-    <row r="381" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="381" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B381" s="33"/>
     </row>
-    <row r="382" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="382" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B382" s="33"/>
     </row>
-    <row r="383" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="383" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B383" s="33"/>
     </row>
-    <row r="384" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="384" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B384" s="33"/>
     </row>
-    <row r="385" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="385" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B385" s="33"/>
     </row>
-    <row r="386" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="386" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B386" s="33"/>
     </row>
-    <row r="387" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="387" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B387" s="33"/>
     </row>
-    <row r="388" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="388" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B388" s="33"/>
     </row>
-    <row r="389" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="389" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B389" s="33"/>
     </row>
-    <row r="390" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="390" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B390" s="33"/>
     </row>
-    <row r="391" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="391" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B391" s="33"/>
     </row>
-    <row r="392" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="392" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B392" s="33"/>
     </row>
-    <row r="393" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="393" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B393" s="33"/>
     </row>
-    <row r="394" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="394" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B394" s="33"/>
     </row>
-    <row r="395" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="395" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B395" s="33"/>
     </row>
-    <row r="396" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="396" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B396" s="33"/>
     </row>
-    <row r="397" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="397" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B397" s="33"/>
     </row>
-    <row r="398" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="398" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B398" s="33"/>
     </row>
-    <row r="399" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="399" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B399" s="33"/>
     </row>
-    <row r="400" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="400" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B400" s="33"/>
     </row>
-    <row r="401" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="401" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B401" s="33"/>
     </row>
-    <row r="402" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="402" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B402" s="33"/>
     </row>
-    <row r="403" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="403" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B403" s="33"/>
     </row>
-    <row r="404" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="404" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B404" s="33"/>
     </row>
-    <row r="405" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="405" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B405" s="33"/>
     </row>
-    <row r="406" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="406" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B406" s="33"/>
     </row>
-    <row r="407" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="407" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B407" s="33"/>
     </row>
-    <row r="408" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="408" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B408" s="33"/>
     </row>
-    <row r="409" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="409" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B409" s="33"/>
     </row>
-    <row r="410" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="410" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B410" s="33"/>
     </row>
-    <row r="411" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="411" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B411" s="33"/>
     </row>
-    <row r="412" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="412" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B412" s="33"/>
     </row>
-    <row r="413" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="413" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B413" s="33"/>
     </row>
-    <row r="414" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="414" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B414" s="33"/>
     </row>
-    <row r="415" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="415" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B415" s="33"/>
     </row>
-    <row r="416" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="416" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B416" s="33"/>
     </row>
-    <row r="417" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="417" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B417" s="33"/>
     </row>
-    <row r="418" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="418" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B418" s="33"/>
     </row>
-    <row r="419" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="419" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B419" s="33"/>
     </row>
-    <row r="420" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="420" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B420" s="33"/>
     </row>
-    <row r="421" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="421" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B421" s="33"/>
     </row>
-    <row r="422" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="422" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B422" s="33"/>
     </row>
-    <row r="423" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="423" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B423" s="33"/>
     </row>
-    <row r="424" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="424" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B424" s="33"/>
     </row>
-    <row r="425" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="425" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B425" s="33"/>
     </row>
-    <row r="426" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="426" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B426" s="33"/>
     </row>
-    <row r="427" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="427" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B427" s="33"/>
     </row>
-    <row r="428" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="428" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B428" s="33"/>
     </row>
-    <row r="429" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="429" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B429" s="33"/>
     </row>
-    <row r="430" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="430" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B430" s="33"/>
     </row>
-    <row r="431" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="431" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B431" s="33"/>
     </row>
-    <row r="432" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="432" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B432" s="33"/>
     </row>
-    <row r="433" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="433" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B433" s="33"/>
     </row>
-    <row r="434" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="434" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B434" s="33"/>
     </row>
-    <row r="435" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="435" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B435" s="33"/>
     </row>
-    <row r="436" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="436" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B436" s="33"/>
     </row>
-    <row r="437" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="437" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B437" s="33"/>
     </row>
-    <row r="438" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="438" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B438" s="33"/>
     </row>
-    <row r="439" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="439" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B439" s="33"/>
     </row>
-    <row r="440" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="440" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B440" s="33"/>
     </row>
-    <row r="441" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="441" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B441" s="33"/>
     </row>
-    <row r="442" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="442" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B442" s="33"/>
     </row>
-    <row r="443" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="443" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B443" s="33"/>
     </row>
-    <row r="444" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="444" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B444" s="33"/>
     </row>
-    <row r="445" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="445" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B445" s="33"/>
     </row>
-    <row r="446" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="446" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B446" s="33"/>
     </row>
-    <row r="447" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="447" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B447" s="33"/>
     </row>
-    <row r="448" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="448" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B448" s="33"/>
     </row>
-    <row r="449" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="449" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B449" s="33"/>
     </row>
-    <row r="450" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="450" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B450" s="33"/>
     </row>
-    <row r="451" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="451" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B451" s="33"/>
     </row>
-    <row r="452" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="452" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B452" s="33"/>
     </row>
-    <row r="453" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="453" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B453" s="33"/>
     </row>
-    <row r="454" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="454" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B454" s="33"/>
     </row>
-    <row r="455" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="455" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B455" s="33"/>
     </row>
-    <row r="456" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="456" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B456" s="33"/>
     </row>
-    <row r="457" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="457" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B457" s="33"/>
     </row>
-    <row r="458" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="458" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B458" s="33"/>
     </row>
-    <row r="459" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="459" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B459" s="33"/>
     </row>
-    <row r="460" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="460" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B460" s="33"/>
     </row>
-    <row r="461" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="461" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B461" s="33"/>
     </row>
-    <row r="462" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="462" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B462" s="33"/>
     </row>
-    <row r="463" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="463" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B463" s="33"/>
     </row>
-    <row r="464" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="464" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B464" s="33"/>
     </row>
-    <row r="465" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="465" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B465" s="33"/>
     </row>
-    <row r="466" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="466" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B466" s="33"/>
     </row>
-    <row r="467" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="467" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B467" s="33"/>
     </row>
-    <row r="468" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="468" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B468" s="33"/>
     </row>
-    <row r="469" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="469" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B469" s="33"/>
     </row>
-    <row r="470" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="470" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B470" s="33"/>
     </row>
-    <row r="471" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="471" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B471" s="33"/>
     </row>
-    <row r="472" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="472" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B472" s="33"/>
     </row>
-    <row r="473" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="473" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B473" s="33"/>
     </row>
-    <row r="474" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="474" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B474" s="33"/>
     </row>
-    <row r="475" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="475" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B475" s="33"/>
     </row>
-    <row r="476" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="476" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B476" s="33"/>
     </row>
-    <row r="477" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="477" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B477" s="33"/>
     </row>
-    <row r="478" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="478" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B478" s="33"/>
     </row>
-    <row r="479" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="479" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B479" s="33"/>
     </row>
-    <row r="480" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="480" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B480" s="33"/>
     </row>
-    <row r="481" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="481" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B481" s="33"/>
     </row>
-    <row r="482" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="482" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B482" s="33"/>
     </row>
-    <row r="483" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="483" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B483" s="33"/>
     </row>
-    <row r="484" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="484" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B484" s="33"/>
     </row>
-    <row r="485" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="485" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B485" s="33"/>
     </row>
-    <row r="486" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="486" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B486" s="33"/>
     </row>
-    <row r="487" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="487" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B487" s="33"/>
     </row>
-    <row r="488" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="488" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B488" s="33"/>
     </row>
-    <row r="489" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="489" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B489" s="33"/>
     </row>
-    <row r="490" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="490" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B490" s="33"/>
     </row>
-    <row r="491" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="491" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B491" s="33"/>
     </row>
-    <row r="492" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="492" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B492" s="33"/>
     </row>
-    <row r="493" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="493" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B493" s="33"/>
     </row>
-    <row r="494" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="494" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B494" s="33"/>
     </row>
-    <row r="495" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="495" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B495" s="33"/>
     </row>
-    <row r="496" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="496" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B496" s="33"/>
     </row>
-    <row r="497" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="497" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B497" s="33"/>
     </row>
-    <row r="498" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="498" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B498" s="33"/>
     </row>
-    <row r="499" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="499" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B499" s="33"/>
     </row>
-    <row r="500" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="500" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B500" s="33"/>
     </row>
-    <row r="501" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="501" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B501" s="33"/>
     </row>
-    <row r="502" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="502" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B502" s="33"/>
     </row>
-    <row r="503" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="503" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B503" s="33"/>
     </row>
-    <row r="504" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="504" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B504" s="33"/>
     </row>
-    <row r="505" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="505" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B505" s="33"/>
     </row>
-    <row r="506" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="506" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B506" s="33"/>
     </row>
-    <row r="507" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="507" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B507" s="33"/>
     </row>
-    <row r="508" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="508" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B508" s="33"/>
     </row>
-    <row r="509" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="509" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B509" s="33"/>
     </row>
-    <row r="510" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="510" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B510" s="33"/>
     </row>
-    <row r="511" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="511" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B511" s="33"/>
     </row>
-    <row r="512" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="512" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B512" s="33"/>
     </row>
-    <row r="513" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="513" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B513" s="33"/>
     </row>
-    <row r="514" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="514" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B514" s="33"/>
     </row>
-    <row r="515" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="515" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B515" s="33"/>
     </row>
-    <row r="516" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="516" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B516" s="33"/>
     </row>
-    <row r="517" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="517" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B517" s="33"/>
     </row>
-    <row r="518" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="518" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B518" s="33"/>
     </row>
-    <row r="519" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="519" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B519" s="33"/>
     </row>
-    <row r="520" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="520" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B520" s="33"/>
     </row>
-    <row r="521" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="521" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B521" s="33"/>
     </row>
-    <row r="522" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="522" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B522" s="33"/>
     </row>
-    <row r="523" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="523" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B523" s="33"/>
     </row>
-    <row r="524" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="524" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B524" s="33"/>
     </row>
-    <row r="525" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="525" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B525" s="33"/>
     </row>
-    <row r="526" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="526" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B526" s="33"/>
     </row>
-    <row r="527" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="527" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B527" s="33"/>
     </row>
-    <row r="528" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="528" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B528" s="33"/>
     </row>
-    <row r="529" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="529" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B529" s="33"/>
     </row>
-    <row r="530" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="530" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B530" s="33"/>
     </row>
-    <row r="531" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="531" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B531" s="33"/>
     </row>
-    <row r="532" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="532" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B532" s="33"/>
     </row>
-    <row r="533" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="533" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B533" s="33"/>
     </row>
-    <row r="534" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="534" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B534" s="33"/>
     </row>
-    <row r="535" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="535" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B535" s="33"/>
     </row>
-    <row r="536" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="536" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B536" s="33"/>
     </row>
-    <row r="537" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="537" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B537" s="33"/>
     </row>
-    <row r="538" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="538" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B538" s="33"/>
     </row>
-    <row r="539" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="539" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B539" s="33"/>
     </row>
-    <row r="540" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="540" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B540" s="33"/>
     </row>
-    <row r="541" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="541" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B541" s="33"/>
     </row>
-    <row r="542" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="542" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B542" s="33"/>
     </row>
-    <row r="543" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="543" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B543" s="33"/>
     </row>
-    <row r="544" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="544" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B544" s="33"/>
     </row>
-    <row r="545" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="545" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B545" s="33"/>
     </row>
-    <row r="546" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="546" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B546" s="33"/>
     </row>
-    <row r="547" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="547" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B547" s="33"/>
     </row>
-    <row r="548" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="548" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B548" s="33"/>
     </row>
-    <row r="549" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="549" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B549" s="33"/>
     </row>
-    <row r="550" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="550" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B550" s="33"/>
     </row>
-    <row r="551" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="551" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B551" s="33"/>
     </row>
-    <row r="552" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="552" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B552" s="33"/>
     </row>
-    <row r="553" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="553" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B553" s="33"/>
     </row>
-    <row r="554" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="554" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B554" s="33"/>
     </row>
-    <row r="555" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="555" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B555" s="33"/>
     </row>
-    <row r="556" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="556" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B556" s="33"/>
     </row>
-    <row r="557" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="557" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B557" s="33"/>
     </row>
-    <row r="558" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="558" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B558" s="33"/>
     </row>
-    <row r="559" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="559" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B559" s="33"/>
     </row>
-    <row r="560" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="560" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B560" s="33"/>
     </row>
-    <row r="561" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="561" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B561" s="33"/>
     </row>
-    <row r="562" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="562" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B562" s="33"/>
     </row>
-    <row r="563" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="563" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B563" s="33"/>
     </row>
-    <row r="564" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="564" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B564" s="33"/>
     </row>
-    <row r="565" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="565" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B565" s="33"/>
     </row>
-    <row r="566" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="566" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B566" s="33"/>
     </row>
-    <row r="567" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="567" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B567" s="33"/>
     </row>
-    <row r="568" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="568" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B568" s="33"/>
     </row>
-    <row r="569" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="569" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B569" s="33"/>
     </row>
-    <row r="570" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="570" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B570" s="33"/>
     </row>
-    <row r="571" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="571" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B571" s="33"/>
     </row>
-    <row r="572" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="572" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B572" s="33"/>
     </row>
-    <row r="573" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="573" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B573" s="33"/>
     </row>
-    <row r="574" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="574" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B574" s="33"/>
     </row>
-    <row r="575" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="575" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B575" s="33"/>
     </row>
-    <row r="576" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="576" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B576" s="33"/>
     </row>
-    <row r="577" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="577" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B577" s="33"/>
     </row>
-    <row r="578" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="578" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B578" s="33"/>
     </row>
-    <row r="579" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="579" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B579" s="33"/>
     </row>
-    <row r="580" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="580" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B580" s="33"/>
     </row>
-    <row r="581" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="581" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B581" s="33"/>
     </row>
-    <row r="582" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="582" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B582" s="33"/>
     </row>
-    <row r="583" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="583" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B583" s="33"/>
     </row>
-    <row r="584" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="584" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B584" s="33"/>
     </row>
-    <row r="585" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="585" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B585" s="33"/>
     </row>
-    <row r="586" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="586" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B586" s="33"/>
     </row>
-    <row r="587" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="587" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B587" s="33"/>
     </row>
-    <row r="588" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="588" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B588" s="33"/>
     </row>
-    <row r="589" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="589" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B589" s="33"/>
     </row>
-    <row r="590" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="590" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B590" s="33"/>
     </row>
-    <row r="591" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="591" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B591" s="33"/>
     </row>
-    <row r="592" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="592" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B592" s="33"/>
     </row>
-    <row r="593" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="593" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B593" s="33"/>
     </row>
-    <row r="594" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="594" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B594" s="33"/>
     </row>
-    <row r="595" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="595" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B595" s="33"/>
     </row>
-    <row r="596" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="596" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B596" s="33"/>
     </row>
-    <row r="597" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="597" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B597" s="33"/>
     </row>
-    <row r="598" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="598" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B598" s="33"/>
     </row>
-    <row r="599" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="599" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B599" s="33"/>
     </row>
-    <row r="600" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="600" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B600" s="33"/>
     </row>
-    <row r="601" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="601" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B601" s="33"/>
     </row>
-    <row r="602" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="602" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B602" s="33"/>
     </row>
-    <row r="603" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="603" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B603" s="33"/>
     </row>
-    <row r="604" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="604" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B604" s="33"/>
     </row>
-    <row r="605" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="605" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B605" s="33"/>
     </row>
-    <row r="606" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="606" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B606" s="33"/>
     </row>
-    <row r="607" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="607" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B607" s="33"/>
     </row>
-    <row r="608" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="608" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B608" s="33"/>
     </row>
-    <row r="609" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="609" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B609" s="33"/>
     </row>
-    <row r="610" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="610" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B610" s="33"/>
     </row>
-    <row r="611" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="611" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B611" s="33"/>
     </row>
-    <row r="612" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="612" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B612" s="33"/>
     </row>
-    <row r="613" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="613" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B613" s="33"/>
     </row>
-    <row r="614" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="614" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B614" s="33"/>
     </row>
-    <row r="615" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="615" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B615" s="33"/>
     </row>
-    <row r="616" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="616" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B616" s="33"/>
     </row>
-    <row r="617" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="617" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B617" s="33"/>
     </row>
-    <row r="618" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="618" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B618" s="33"/>
     </row>
-    <row r="619" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="619" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B619" s="33"/>
     </row>
-    <row r="620" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="620" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B620" s="33"/>
     </row>
-    <row r="621" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="621" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B621" s="33"/>
     </row>
-    <row r="622" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="622" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B622" s="33"/>
     </row>
-    <row r="623" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="623" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B623" s="33"/>
     </row>
-    <row r="624" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="624" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B624" s="33"/>
     </row>
-    <row r="625" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="625" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B625" s="33"/>
     </row>
-    <row r="626" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="626" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B626" s="33"/>
     </row>
-    <row r="627" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="627" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B627" s="33"/>
     </row>
-    <row r="628" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="628" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B628" s="33"/>
     </row>
-    <row r="629" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="629" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B629" s="33"/>
     </row>
-    <row r="630" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="630" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B630" s="33"/>
     </row>
-    <row r="631" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="631" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B631" s="33"/>
     </row>
-    <row r="632" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="632" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B632" s="33"/>
     </row>
-    <row r="633" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="633" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B633" s="33"/>
     </row>
-    <row r="634" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="634" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B634" s="33"/>
     </row>
-    <row r="635" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="635" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B635" s="33"/>
     </row>
-    <row r="636" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="636" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B636" s="33"/>
     </row>
-    <row r="637" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="637" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B637" s="33"/>
     </row>
-    <row r="638" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="638" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B638" s="33"/>
     </row>
-    <row r="639" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="639" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B639" s="33"/>
     </row>
-    <row r="640" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="640" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B640" s="33"/>
     </row>
-    <row r="641" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="641" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B641" s="33"/>
     </row>
-    <row r="642" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="642" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B642" s="33"/>
     </row>
-    <row r="643" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="643" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B643" s="33"/>
     </row>
-    <row r="644" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="644" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B644" s="33"/>
     </row>
-    <row r="645" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="645" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B645" s="33"/>
     </row>
-    <row r="646" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="646" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B646" s="33"/>
     </row>
-    <row r="647" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="647" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B647" s="33"/>
     </row>
-    <row r="648" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="648" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B648" s="33"/>
     </row>
-    <row r="649" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="649" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B649" s="33"/>
     </row>
-    <row r="650" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="650" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B650" s="33"/>
     </row>
-    <row r="651" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="651" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B651" s="33"/>
     </row>
-    <row r="652" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="652" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B652" s="33"/>
     </row>
-    <row r="653" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="653" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B653" s="33"/>
     </row>
-    <row r="654" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="654" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B654" s="33"/>
     </row>
-    <row r="655" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="655" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B655" s="33"/>
     </row>
-    <row r="656" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="656" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B656" s="33"/>
     </row>
-    <row r="657" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="657" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B657" s="33"/>
     </row>
-    <row r="658" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="658" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B658" s="33"/>
     </row>
-    <row r="659" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="659" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B659" s="33"/>
     </row>
-    <row r="660" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="660" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B660" s="33"/>
     </row>
-    <row r="661" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="661" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B661" s="33"/>
     </row>
-    <row r="662" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="662" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B662" s="33"/>
     </row>
-    <row r="663" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="663" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B663" s="33"/>
     </row>
-    <row r="664" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="664" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B664" s="33"/>
     </row>
-    <row r="665" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="665" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B665" s="33"/>
     </row>
-    <row r="666" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="666" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B666" s="33"/>
     </row>
-    <row r="667" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="667" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B667" s="33"/>
     </row>
   </sheetData>
@@ -6332,16 +6332,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15.5546875" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="s">
         <v>1</v>
       </c>
@@ -6350,7 +6350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -6361,7 +6361,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -6372,7 +6372,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -6380,18 +6380,18 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -6406,20 +6406,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D74D41B-283E-4F55-BA94-91EF2EF7E1E9}">
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A25" sqref="A25:H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="12.88671875" customWidth="1"/>
-    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B1" s="46"/>
       <c r="C1" s="46"/>
@@ -6429,9 +6429,9 @@
       <c r="G1" s="46"/>
       <c r="H1" s="46"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" s="25">
         <v>6</v>
@@ -6452,12 +6452,12 @@
         <v>1</v>
       </c>
       <c r="H2" s="25" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="47" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B3" s="48"/>
       <c r="C3" s="48"/>
@@ -6467,35 +6467,35 @@
       <c r="G3" s="48"/>
       <c r="H3" s="49"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E4" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G4" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H4" s="25" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="46" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B7" s="46"/>
       <c r="C7" s="46"/>
@@ -6505,9 +6505,9 @@
       <c r="G7" s="46"/>
       <c r="H7" s="46"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B8" s="25">
         <v>6</v>
@@ -6528,12 +6528,12 @@
         <v>1</v>
       </c>
       <c r="H8" s="25" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="47" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B9" s="48"/>
       <c r="C9" s="48"/>
@@ -6543,35 +6543,35 @@
       <c r="G9" s="48"/>
       <c r="H9" s="49"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F10" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G10" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H10" s="25" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="46" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B13" s="46"/>
       <c r="C13" s="46"/>
@@ -6581,9 +6581,9 @@
       <c r="G13" s="46"/>
       <c r="H13" s="46"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B14" s="25">
         <v>6</v>
@@ -6604,12 +6604,12 @@
         <v>1</v>
       </c>
       <c r="H14" s="25" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="47" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B15" s="48"/>
       <c r="C15" s="48"/>
@@ -6619,35 +6619,35 @@
       <c r="G15" s="48"/>
       <c r="H15" s="49"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E16" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F16" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G16" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H16" s="25" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="46" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B19" s="46"/>
       <c r="C19" s="46"/>
@@ -6657,9 +6657,9 @@
       <c r="G19" s="46"/>
       <c r="H19" s="46"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B20" s="25">
         <v>6</v>
@@ -6680,12 +6680,12 @@
         <v>1</v>
       </c>
       <c r="H20" s="25" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="47" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B21" s="48"/>
       <c r="C21" s="48"/>
@@ -6695,35 +6695,35 @@
       <c r="G21" s="48"/>
       <c r="H21" s="49"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E22" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F22" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G22" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H22" s="25" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="46" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B25" s="46"/>
       <c r="C25" s="46"/>
@@ -6733,9 +6733,9 @@
       <c r="G25" s="46"/>
       <c r="H25" s="46"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B26" s="6">
         <v>6</v>
@@ -6756,10 +6756,10 @@
         <v>1</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="24">
         <v>0</v>
       </c>
@@ -6770,50 +6770,50 @@
         <v>0</v>
       </c>
       <c r="D27" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E27" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="6" t="s">
+      <c r="B28" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="H28" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B28" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="E28" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="G28" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="H28" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="46" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B31" s="46"/>
       <c r="C31" s="46"/>
@@ -6823,9 +6823,9 @@
       <c r="G31" s="46"/>
       <c r="H31" s="46"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B32" s="6">
         <v>6</v>
@@ -6846,58 +6846,58 @@
         <v>1</v>
       </c>
       <c r="H32" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="6">
+        <v>0</v>
+      </c>
+      <c r="B33" s="6">
+        <v>0</v>
+      </c>
+      <c r="C33" s="6">
+        <v>0</v>
+      </c>
+      <c r="D33" s="6">
+        <v>0</v>
+      </c>
+      <c r="E33" s="46" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="6">
-        <v>0</v>
-      </c>
-      <c r="B33" s="6">
-        <v>0</v>
-      </c>
-      <c r="C33" s="6">
-        <v>0</v>
-      </c>
-      <c r="D33" s="6">
-        <v>0</v>
-      </c>
-      <c r="E33" s="46" t="s">
-        <v>64</v>
       </c>
       <c r="F33" s="46"/>
       <c r="G33" s="46"/>
       <c r="H33" s="46"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E34" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="F34" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="G34" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="H34" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="E34" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G34" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="H34" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B37" s="46"/>
       <c r="C37" s="46"/>
@@ -6907,9 +6907,9 @@
       <c r="G37" s="46"/>
       <c r="H37" s="46"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B38" s="20">
         <v>6</v>
@@ -6930,10 +6930,10 @@
         <v>1</v>
       </c>
       <c r="H38" s="20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="20">
         <v>0</v>
       </c>
@@ -6941,48 +6941,48 @@
         <v>0</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D39" s="20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H39" s="20" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B40" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="C40" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D40" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="E40" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="F40" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="G40" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="H40" s="20" t="s">
         <v>69</v>
-      </c>
-      <c r="B40" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="C40" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="D40" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="E40" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="F40" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="G40" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="H40" s="20" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleanup, ready for specific component values.
</commit_message>
<xml_diff>
--- a/Doc/Encodings.xlsx
+++ b/Doc/Encodings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pschilk\home\Repos\psMCU\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D303F92-7564-4DDD-A880-7E379E713497}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEEE780D-79A9-4D47-ACE5-A07B0C008ABE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inst Decoding" sheetId="2" r:id="rId1"/>
@@ -197,9 +197,6 @@
     <t>0x0E(A),0x0F(B)</t>
   </si>
   <si>
-    <t>0x10(B),0x11(B)</t>
-  </si>
-  <si>
     <t>0x12(A),0x13(B)</t>
   </si>
   <si>
@@ -272,9 +269,6 @@
     <t>LD[A/B]</t>
   </si>
   <si>
-    <t>LIT</t>
-  </si>
-  <si>
     <t>A=0</t>
   </si>
   <si>
@@ -432,6 +426,12 @@
   </si>
   <si>
     <t>XOR</t>
+  </si>
+  <si>
+    <t>0x10(A),0x11(B)</t>
+  </si>
+  <si>
+    <t>LIT[A/B]</t>
   </si>
 </sst>
 </file>
@@ -2312,8 +2312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59778E2C-D2B8-41E1-8336-5F65E1F1812B}">
   <dimension ref="A1:R667"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2330,7 +2330,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C1" s="2">
         <v>15</v>
@@ -2371,37 +2371,37 @@
     </row>
     <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="H2" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="I2" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="K2" s="13" t="s">
         <v>127</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="C2" s="30" t="s">
-        <v>126</v>
-      </c>
-      <c r="D2" s="30" t="s">
-        <v>126</v>
-      </c>
-      <c r="E2" s="30" t="s">
-        <v>126</v>
-      </c>
-      <c r="F2" s="30" t="s">
-        <v>126</v>
-      </c>
-      <c r="G2" s="30" t="s">
-        <v>126</v>
-      </c>
-      <c r="H2" s="30" t="s">
-        <v>126</v>
-      </c>
-      <c r="I2" s="30" t="s">
-        <v>126</v>
-      </c>
-      <c r="J2" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="K2" s="13" t="s">
-        <v>129</v>
       </c>
       <c r="L2" s="13">
         <v>128</v>
@@ -2418,7 +2418,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C3" s="5">
         <v>1</v>
@@ -2437,7 +2437,7 @@
         <v>50</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="L3" s="13">
         <v>32</v>
@@ -2454,7 +2454,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C4" s="8">
         <v>1</v>
@@ -2473,7 +2473,7 @@
         <v>49</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="L4" s="13">
         <v>32</v>
@@ -2490,7 +2490,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C5" s="8">
         <v>0</v>
@@ -2502,7 +2502,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G5" s="43" t="s">
         <v>10</v>
@@ -2513,7 +2513,7 @@
         <v>48</v>
       </c>
       <c r="K5" s="13" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L5" s="13">
         <v>16</v>
@@ -2530,7 +2530,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C6" s="8">
         <v>0</v>
@@ -2542,7 +2542,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G6" s="43" t="s">
         <v>10</v>
@@ -2553,7 +2553,7 @@
         <v>47</v>
       </c>
       <c r="K6" s="13" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="L6" s="13">
         <v>16</v>
@@ -2567,10 +2567,10 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="36" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C7" s="8">
         <v>0</v>
@@ -2594,7 +2594,7 @@
         <v>1</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K7" s="13" t="s">
         <v>28</v>
@@ -2611,10 +2611,10 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C8" s="8">
         <v>0</v>
@@ -2638,7 +2638,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="K8" s="13" t="s">
         <v>28</v>
@@ -2655,10 +2655,10 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="37" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C9" s="8">
         <v>0</v>
@@ -2682,10 +2682,10 @@
         <v>1</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="K9" s="13" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L9" s="13">
         <v>1</v>
@@ -2699,10 +2699,10 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="37" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C10" s="8">
         <v>0</v>
@@ -2726,10 +2726,10 @@
         <v>0</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="K10" s="13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="L10" s="13">
         <v>1</v>
@@ -2743,10 +2743,10 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="37" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C11" s="8">
         <v>0</v>
@@ -2770,10 +2770,10 @@
         <v>1</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="K11" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L11" s="13">
         <v>1</v>
@@ -2787,10 +2787,10 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="37" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C12" s="8">
         <v>0</v>
@@ -2814,10 +2814,10 @@
         <v>0</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K12" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L12" s="13">
         <v>1</v>
@@ -2831,37 +2831,37 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="B13" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0</v>
+      </c>
+      <c r="D13" s="27">
+        <v>0</v>
+      </c>
+      <c r="E13" s="29">
+        <v>1</v>
+      </c>
+      <c r="F13" s="9">
+        <v>1</v>
+      </c>
+      <c r="G13" s="26">
+        <v>0</v>
+      </c>
+      <c r="H13" s="26">
+        <v>0</v>
+      </c>
+      <c r="I13" s="27">
+        <v>1</v>
+      </c>
+      <c r="J13" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="B13" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="C13" s="8">
-        <v>0</v>
-      </c>
-      <c r="D13" s="27">
-        <v>0</v>
-      </c>
-      <c r="E13" s="29">
-        <v>1</v>
-      </c>
-      <c r="F13" s="9">
-        <v>1</v>
-      </c>
-      <c r="G13" s="26">
-        <v>0</v>
-      </c>
-      <c r="H13" s="26">
-        <v>0</v>
-      </c>
-      <c r="I13" s="27">
-        <v>1</v>
-      </c>
-      <c r="J13" s="13" t="s">
-        <v>114</v>
-      </c>
       <c r="K13" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L13" s="13">
         <v>1</v>
@@ -2875,34 +2875,34 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="35" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B14" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0</v>
+      </c>
+      <c r="D14" s="22">
+        <v>0</v>
+      </c>
+      <c r="E14" s="23">
+        <v>1</v>
+      </c>
+      <c r="F14" s="9">
+        <v>1</v>
+      </c>
+      <c r="G14" s="21">
+        <v>0</v>
+      </c>
+      <c r="H14" s="21">
+        <v>0</v>
+      </c>
+      <c r="I14" s="21">
+        <v>0</v>
+      </c>
+      <c r="J14" s="13" t="s">
         <v>88</v>
-      </c>
-      <c r="C14" s="8">
-        <v>0</v>
-      </c>
-      <c r="D14" s="22">
-        <v>0</v>
-      </c>
-      <c r="E14" s="23">
-        <v>1</v>
-      </c>
-      <c r="F14" s="9">
-        <v>1</v>
-      </c>
-      <c r="G14" s="21">
-        <v>0</v>
-      </c>
-      <c r="H14" s="21">
-        <v>0</v>
-      </c>
-      <c r="I14" s="21">
-        <v>0</v>
-      </c>
-      <c r="J14" s="13" t="s">
-        <v>90</v>
       </c>
       <c r="K14" s="13" t="s">
         <v>45</v>
@@ -2922,7 +2922,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C15" s="8">
         <v>0</v>
@@ -2964,7 +2964,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C16" s="8">
         <v>0</v>
@@ -2991,7 +2991,7 @@
         <v>53</v>
       </c>
       <c r="K16" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L16" s="13">
         <v>2</v>
@@ -3008,7 +3008,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C17" s="8">
         <v>0</v>
@@ -3035,7 +3035,7 @@
         <v>52</v>
       </c>
       <c r="K17" s="13" t="s">
-        <v>56</v>
+        <v>133</v>
       </c>
       <c r="L17" s="13">
         <v>2</v>
@@ -3052,7 +3052,7 @@
         <v>14</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>81</v>
+        <v>134</v>
       </c>
       <c r="C18" s="8">
         <v>0</v>
@@ -3096,7 +3096,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C19" s="8">
         <v>0</v>
@@ -3140,7 +3140,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C20" s="8">
         <v>0</v>
@@ -3184,7 +3184,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C21" s="8">
         <v>0</v>
@@ -3228,7 +3228,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C22" s="8">
         <v>0</v>
@@ -3272,7 +3272,7 @@
         <v>54</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C23" s="8">
         <v>0</v>
@@ -3316,7 +3316,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C24" s="8">
         <v>0</v>
@@ -3357,10 +3357,10 @@
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C25" s="8">
         <v>0</v>
@@ -3401,10 +3401,10 @@
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C26" s="8">
         <v>0</v>
@@ -3489,10 +3489,10 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C28" s="8">
         <v>0</v>
@@ -3533,10 +3533,10 @@
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C29" s="8">
         <v>0</v>
@@ -3580,7 +3580,7 @@
         <v>24</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C30" s="8">
         <v>0</v>
@@ -6332,7 +6332,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
@@ -6380,7 +6380,7 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -6419,7 +6419,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="46" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B1" s="46"/>
       <c r="C1" s="46"/>
@@ -6431,7 +6431,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="25">
         <v>6</v>
@@ -6452,12 +6452,12 @@
         <v>1</v>
       </c>
       <c r="H2" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="47" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B3" s="48"/>
       <c r="C3" s="48"/>
@@ -6469,33 +6469,33 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E4" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G4" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H4" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="46" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B7" s="46"/>
       <c r="C7" s="46"/>
@@ -6507,7 +6507,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" s="25">
         <v>6</v>
@@ -6528,12 +6528,12 @@
         <v>1</v>
       </c>
       <c r="H8" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="47" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B9" s="48"/>
       <c r="C9" s="48"/>
@@ -6545,33 +6545,33 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F10" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G10" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H10" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="46" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B13" s="46"/>
       <c r="C13" s="46"/>
@@ -6583,7 +6583,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B14" s="25">
         <v>6</v>
@@ -6604,12 +6604,12 @@
         <v>1</v>
       </c>
       <c r="H14" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="47" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B15" s="48"/>
       <c r="C15" s="48"/>
@@ -6621,33 +6621,33 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E16" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F16" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G16" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H16" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="46" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B19" s="46"/>
       <c r="C19" s="46"/>
@@ -6659,7 +6659,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B20" s="25">
         <v>6</v>
@@ -6680,12 +6680,12 @@
         <v>1</v>
       </c>
       <c r="H20" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="47" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B21" s="48"/>
       <c r="C21" s="48"/>
@@ -6697,33 +6697,33 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E22" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F22" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G22" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H22" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="46" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B25" s="46"/>
       <c r="C25" s="46"/>
@@ -6735,7 +6735,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B26" s="6">
         <v>6</v>
@@ -6756,7 +6756,7 @@
         <v>1</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -6770,50 +6770,50 @@
         <v>0</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H28" s="6" t="s">
         <v>68</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E28" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="G28" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="H28" s="6" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="46" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B31" s="46"/>
       <c r="C31" s="46"/>
@@ -6825,7 +6825,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B32" s="6">
         <v>6</v>
@@ -6846,7 +6846,7 @@
         <v>1</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -6863,7 +6863,7 @@
         <v>0</v>
       </c>
       <c r="E33" s="46" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F33" s="46"/>
       <c r="G33" s="46"/>
@@ -6871,33 +6871,33 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E34" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="F34" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="G34" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="H34" s="6" t="s">
         <v>68</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="G34" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="H34" s="6" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="46" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B37" s="46"/>
       <c r="C37" s="46"/>
@@ -6909,7 +6909,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B38" s="20">
         <v>6</v>
@@ -6930,7 +6930,7 @@
         <v>1</v>
       </c>
       <c r="H38" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -6941,48 +6941,48 @@
         <v>0</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D39" s="20" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H39" s="20" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B40" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="C40" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D40" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="E40" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="F40" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="G40" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="H40" s="20" t="s">
         <v>68</v>
-      </c>
-      <c r="B40" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="C40" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="D40" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="E40" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="F40" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="G40" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="H40" s="20" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Logisim: Added Button Interrupt flag
    Also updated StdLib/Documentation
</commit_message>
<xml_diff>
--- a/Doc/Encodings.xlsx
+++ b/Doc/Encodings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pschilk\home\Repos\psMCU\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEEE780D-79A9-4D47-ACE5-A07B0C008ABE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B6CE48-2E70-4A6A-B4D0-FEA63EF54A3F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inst Decoding" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="136">
   <si>
     <t>Operation</t>
   </si>
@@ -432,6 +432,9 @@
   </si>
   <si>
     <t>LIT[A/B]</t>
+  </si>
+  <si>
+    <t>INT_BTN_F</t>
   </si>
 </sst>
 </file>
@@ -497,7 +500,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -694,11 +697,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -806,6 +820,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -837,6 +854,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2312,20 +2332,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59778E2C-D2B8-41E1-8336-5F65E1F1812B}">
   <dimension ref="A1:R667"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" style="19" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" style="15" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" style="15" customWidth="1"/>
-    <col min="12" max="18" width="8.85546875" style="15"/>
+    <col min="1" max="1" width="16.26953125" customWidth="1"/>
+    <col min="2" max="2" width="16.7265625" style="19" customWidth="1"/>
+    <col min="10" max="10" width="11.1796875" style="15" customWidth="1"/>
+    <col min="11" max="11" width="13.81640625" style="15" customWidth="1"/>
+    <col min="12" max="18" width="8.81640625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -2369,7 +2389,7 @@
       <c r="Q1" s="13"/>
       <c r="R1" s="13"/>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="38" t="s">
         <v>125</v>
       </c>
@@ -2413,7 +2433,7 @@
       <c r="Q2" s="13"/>
       <c r="R2" s="13"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="34" t="s">
         <v>6</v>
       </c>
@@ -2426,13 +2446,13 @@
       <c r="D3" s="6">
         <v>1</v>
       </c>
-      <c r="E3" s="39" t="s">
+      <c r="E3" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
       <c r="J3" s="13" t="s">
         <v>50</v>
       </c>
@@ -2449,7 +2469,7 @@
       <c r="Q3" s="14"/>
       <c r="R3" s="14"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="35" t="s">
         <v>8</v>
       </c>
@@ -2462,13 +2482,13 @@
       <c r="D4" s="8">
         <v>0</v>
       </c>
-      <c r="E4" s="41" t="s">
+      <c r="E4" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="42"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
       <c r="J4" s="13" t="s">
         <v>49</v>
       </c>
@@ -2485,7 +2505,7 @@
       <c r="Q4" s="14"/>
       <c r="R4" s="14"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="35" t="s">
         <v>9</v>
       </c>
@@ -2504,11 +2524,11 @@
       <c r="F5" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="G5" s="43" t="s">
+      <c r="G5" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="44"/>
       <c r="J5" s="13" t="s">
         <v>48</v>
       </c>
@@ -2525,7 +2545,7 @@
       <c r="Q5" s="13"/>
       <c r="R5" s="13"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="35" t="s">
         <v>11</v>
       </c>
@@ -2544,11 +2564,11 @@
       <c r="F6" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="G6" s="43" t="s">
+      <c r="G6" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
       <c r="J6" s="13" t="s">
         <v>47</v>
       </c>
@@ -2565,7 +2585,7 @@
       <c r="Q6" s="13"/>
       <c r="R6" s="13"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" s="36" t="s">
         <v>111</v>
       </c>
@@ -2609,7 +2629,7 @@
       <c r="Q7" s="13"/>
       <c r="R7" s="13"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" s="36" t="s">
         <v>111</v>
       </c>
@@ -2653,7 +2673,7 @@
       <c r="Q8" s="13"/>
       <c r="R8" s="13"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" s="37" t="s">
         <v>106</v>
       </c>
@@ -2697,7 +2717,7 @@
       <c r="Q9" s="13"/>
       <c r="R9" s="13"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" s="37" t="s">
         <v>107</v>
       </c>
@@ -2741,7 +2761,7 @@
       <c r="Q10" s="13"/>
       <c r="R10" s="13"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" s="37" t="s">
         <v>108</v>
       </c>
@@ -2785,7 +2805,7 @@
       <c r="Q11" s="13"/>
       <c r="R11" s="13"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" s="37" t="s">
         <v>109</v>
       </c>
@@ -2829,7 +2849,7 @@
       <c r="Q12" s="13"/>
       <c r="R12" s="13"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" s="37" t="s">
         <v>110</v>
       </c>
@@ -2873,7 +2893,7 @@
       <c r="Q13" s="13"/>
       <c r="R13" s="13"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" s="35" t="s">
         <v>87</v>
       </c>
@@ -2917,7 +2937,7 @@
       <c r="Q14" s="13"/>
       <c r="R14" s="13"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" s="35" t="s">
         <v>12</v>
       </c>
@@ -2939,10 +2959,10 @@
       <c r="G15" s="6">
         <v>1</v>
       </c>
-      <c r="H15" s="44" t="s">
+      <c r="H15" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="I15" s="44"/>
+      <c r="I15" s="45"/>
       <c r="J15" s="13" t="s">
         <v>42</v>
       </c>
@@ -2959,7 +2979,7 @@
       <c r="Q15" s="13"/>
       <c r="R15" s="13"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>15</v>
       </c>
@@ -3003,7 +3023,7 @@
       <c r="Q16" s="13"/>
       <c r="R16" s="13"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>17</v>
       </c>
@@ -3047,7 +3067,7 @@
       <c r="Q17" s="13"/>
       <c r="R17" s="13"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>14</v>
       </c>
@@ -3091,7 +3111,7 @@
       <c r="Q18" s="13"/>
       <c r="R18" s="13"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>18</v>
       </c>
@@ -3135,7 +3155,7 @@
       <c r="Q19" s="13"/>
       <c r="R19" s="13"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>19</v>
       </c>
@@ -3179,7 +3199,7 @@
       <c r="Q20" s="13"/>
       <c r="R20" s="13"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
         <v>20</v>
       </c>
@@ -3223,7 +3243,7 @@
       <c r="Q21" s="13"/>
       <c r="R21" s="13"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>21</v>
       </c>
@@ -3267,7 +3287,7 @@
       <c r="Q22" s="13"/>
       <c r="R22" s="13"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>54</v>
       </c>
@@ -3311,7 +3331,7 @@
       <c r="Q23" s="13"/>
       <c r="R23" s="13"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
         <v>22</v>
       </c>
@@ -3355,7 +3375,7 @@
       <c r="Q24" s="13"/>
       <c r="R24" s="13"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
         <v>83</v>
       </c>
@@ -3399,7 +3419,7 @@
       <c r="Q25" s="13"/>
       <c r="R25" s="13"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
         <v>129</v>
       </c>
@@ -3443,7 +3463,7 @@
       <c r="Q26" s="13"/>
       <c r="R26" s="13"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
         <v>23</v>
       </c>
@@ -3487,7 +3507,7 @@
       <c r="Q27" s="13"/>
       <c r="R27" s="13"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A28" s="7" t="s">
         <v>104</v>
       </c>
@@ -3531,7 +3551,7 @@
       <c r="Q28" s="13"/>
       <c r="R28" s="13"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A29" s="7" t="s">
         <v>105</v>
       </c>
@@ -3575,7 +3595,7 @@
       <c r="Q29" s="13"/>
       <c r="R29" s="13"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A30" s="7" t="s">
         <v>24</v>
       </c>
@@ -3619,7 +3639,7 @@
       <c r="Q30" s="13"/>
       <c r="R30" s="13"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A31" s="7" t="s">
         <v>25</v>
       </c>
@@ -3663,7 +3683,7 @@
       <c r="Q31" s="13"/>
       <c r="R31" s="13"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A32" s="7" t="s">
         <v>26</v>
       </c>
@@ -3707,1909 +3727,1909 @@
       <c r="Q32" s="13"/>
       <c r="R32" s="13"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B33" s="32"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B34" s="33"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B35" s="33"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B36" s="33"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B37" s="33"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B38" s="33"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B39" s="33"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B40" s="33"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B41" s="33"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B42" s="33"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B43" s="33"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B44" s="33"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B45" s="33"/>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B46" s="33"/>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B47" s="33"/>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B48" s="33"/>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B49" s="33"/>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B50" s="33"/>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B51" s="33"/>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B52" s="33"/>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B53" s="33"/>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B54" s="33"/>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B55" s="33"/>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B56" s="33"/>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B57" s="33"/>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B58" s="33"/>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B59" s="33"/>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B60" s="33"/>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B61" s="33"/>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B62" s="33"/>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B63" s="33"/>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B64" s="33"/>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B65" s="33"/>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B66" s="33"/>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B67" s="33"/>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B68" s="33"/>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B69" s="33"/>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B70" s="33"/>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B71" s="33"/>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B72" s="33"/>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B73" s="33"/>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B74" s="33"/>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B75" s="33"/>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B76" s="33"/>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B77" s="33"/>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B78" s="33"/>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B79" s="33"/>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B80" s="33"/>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B81" s="33"/>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B82" s="33"/>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B83" s="33"/>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B84" s="33"/>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B85" s="33"/>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B86" s="33"/>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B87" s="33"/>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B88" s="33"/>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B89" s="33"/>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B90" s="33"/>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B91" s="33"/>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B92" s="33"/>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B93" s="33"/>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B94" s="33"/>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B95" s="33"/>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B96" s="33"/>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B97" s="33"/>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B98" s="33"/>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B99" s="33"/>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B100" s="33"/>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B101" s="33"/>
     </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B102" s="33"/>
     </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B103" s="33"/>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B104" s="33"/>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B105" s="33"/>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B106" s="33"/>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B107" s="33"/>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B108" s="33"/>
     </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B109" s="33"/>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B110" s="33"/>
     </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B111" s="33"/>
     </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B112" s="33"/>
     </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B113" s="33"/>
     </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B114" s="33"/>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B115" s="33"/>
     </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B116" s="33"/>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B117" s="33"/>
     </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B118" s="33"/>
     </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B119" s="33"/>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B120" s="33"/>
     </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B121" s="33"/>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B122" s="33"/>
     </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B123" s="33"/>
     </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B124" s="33"/>
     </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B125" s="33"/>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B126" s="33"/>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B127" s="33"/>
     </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B128" s="33"/>
     </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B129" s="33"/>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B130" s="33"/>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B131" s="33"/>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B132" s="33"/>
     </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B133" s="33"/>
     </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B134" s="33"/>
     </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B135" s="33"/>
     </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B136" s="33"/>
     </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B137" s="33"/>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B138" s="33"/>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B139" s="33"/>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B140" s="33"/>
     </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B141" s="33"/>
     </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B142" s="33"/>
     </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B143" s="33"/>
     </row>
-    <row r="144" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B144" s="33"/>
     </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B145" s="33"/>
     </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B146" s="33"/>
     </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B147" s="33"/>
     </row>
-    <row r="148" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B148" s="33"/>
     </row>
-    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B149" s="33"/>
     </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B150" s="33"/>
     </row>
-    <row r="151" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B151" s="33"/>
     </row>
-    <row r="152" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B152" s="33"/>
     </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B153" s="33"/>
     </row>
-    <row r="154" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B154" s="33"/>
     </row>
-    <row r="155" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B155" s="33"/>
     </row>
-    <row r="156" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B156" s="33"/>
     </row>
-    <row r="157" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B157" s="33"/>
     </row>
-    <row r="158" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B158" s="33"/>
     </row>
-    <row r="159" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B159" s="33"/>
     </row>
-    <row r="160" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B160" s="33"/>
     </row>
-    <row r="161" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B161" s="33"/>
     </row>
-    <row r="162" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B162" s="33"/>
     </row>
-    <row r="163" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B163" s="33"/>
     </row>
-    <row r="164" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B164" s="33"/>
     </row>
-    <row r="165" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B165" s="33"/>
     </row>
-    <row r="166" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B166" s="33"/>
     </row>
-    <row r="167" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B167" s="33"/>
     </row>
-    <row r="168" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B168" s="33"/>
     </row>
-    <row r="169" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B169" s="33"/>
     </row>
-    <row r="170" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B170" s="33"/>
     </row>
-    <row r="171" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B171" s="33"/>
     </row>
-    <row r="172" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B172" s="33"/>
     </row>
-    <row r="173" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B173" s="33"/>
     </row>
-    <row r="174" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B174" s="33"/>
     </row>
-    <row r="175" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B175" s="33"/>
     </row>
-    <row r="176" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B176" s="33"/>
     </row>
-    <row r="177" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B177" s="33"/>
     </row>
-    <row r="178" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B178" s="33"/>
     </row>
-    <row r="179" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B179" s="33"/>
     </row>
-    <row r="180" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B180" s="33"/>
     </row>
-    <row r="181" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B181" s="33"/>
     </row>
-    <row r="182" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B182" s="33"/>
     </row>
-    <row r="183" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B183" s="33"/>
     </row>
-    <row r="184" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B184" s="33"/>
     </row>
-    <row r="185" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B185" s="33"/>
     </row>
-    <row r="186" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B186" s="33"/>
     </row>
-    <row r="187" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B187" s="33"/>
     </row>
-    <row r="188" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B188" s="33"/>
     </row>
-    <row r="189" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B189" s="33"/>
     </row>
-    <row r="190" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B190" s="33"/>
     </row>
-    <row r="191" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B191" s="33"/>
     </row>
-    <row r="192" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B192" s="33"/>
     </row>
-    <row r="193" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B193" s="33"/>
     </row>
-    <row r="194" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B194" s="33"/>
     </row>
-    <row r="195" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B195" s="33"/>
     </row>
-    <row r="196" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B196" s="33"/>
     </row>
-    <row r="197" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B197" s="33"/>
     </row>
-    <row r="198" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B198" s="33"/>
     </row>
-    <row r="199" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B199" s="33"/>
     </row>
-    <row r="200" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B200" s="33"/>
     </row>
-    <row r="201" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B201" s="33"/>
     </row>
-    <row r="202" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B202" s="33"/>
     </row>
-    <row r="203" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B203" s="33"/>
     </row>
-    <row r="204" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B204" s="33"/>
     </row>
-    <row r="205" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B205" s="33"/>
     </row>
-    <row r="206" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B206" s="33"/>
     </row>
-    <row r="207" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B207" s="33"/>
     </row>
-    <row r="208" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B208" s="33"/>
     </row>
-    <row r="209" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B209" s="33"/>
     </row>
-    <row r="210" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B210" s="33"/>
     </row>
-    <row r="211" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B211" s="33"/>
     </row>
-    <row r="212" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="212" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B212" s="33"/>
     </row>
-    <row r="213" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="213" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B213" s="33"/>
     </row>
-    <row r="214" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="214" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B214" s="33"/>
     </row>
-    <row r="215" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="215" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B215" s="33"/>
     </row>
-    <row r="216" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="216" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B216" s="33"/>
     </row>
-    <row r="217" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="217" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B217" s="33"/>
     </row>
-    <row r="218" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="218" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B218" s="33"/>
     </row>
-    <row r="219" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="219" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B219" s="33"/>
     </row>
-    <row r="220" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="220" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B220" s="33"/>
     </row>
-    <row r="221" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="221" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B221" s="33"/>
     </row>
-    <row r="222" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="222" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B222" s="33"/>
     </row>
-    <row r="223" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="223" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B223" s="33"/>
     </row>
-    <row r="224" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="224" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B224" s="33"/>
     </row>
-    <row r="225" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="225" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B225" s="33"/>
     </row>
-    <row r="226" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="226" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B226" s="33"/>
     </row>
-    <row r="227" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="227" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B227" s="33"/>
     </row>
-    <row r="228" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="228" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B228" s="33"/>
     </row>
-    <row r="229" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="229" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B229" s="33"/>
     </row>
-    <row r="230" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="230" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B230" s="33"/>
     </row>
-    <row r="231" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="231" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B231" s="33"/>
     </row>
-    <row r="232" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="232" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B232" s="33"/>
     </row>
-    <row r="233" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="233" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B233" s="33"/>
     </row>
-    <row r="234" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="234" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B234" s="33"/>
     </row>
-    <row r="235" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="235" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B235" s="33"/>
     </row>
-    <row r="236" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="236" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B236" s="33"/>
     </row>
-    <row r="237" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="237" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B237" s="33"/>
     </row>
-    <row r="238" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="238" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B238" s="33"/>
     </row>
-    <row r="239" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="239" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B239" s="33"/>
     </row>
-    <row r="240" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="240" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B240" s="33"/>
     </row>
-    <row r="241" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="241" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B241" s="33"/>
     </row>
-    <row r="242" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="242" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B242" s="33"/>
     </row>
-    <row r="243" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="243" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B243" s="33"/>
     </row>
-    <row r="244" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="244" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B244" s="33"/>
     </row>
-    <row r="245" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="245" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B245" s="33"/>
     </row>
-    <row r="246" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="246" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B246" s="33"/>
     </row>
-    <row r="247" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="247" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B247" s="33"/>
     </row>
-    <row r="248" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="248" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B248" s="33"/>
     </row>
-    <row r="249" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="249" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B249" s="33"/>
     </row>
-    <row r="250" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="250" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B250" s="33"/>
     </row>
-    <row r="251" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="251" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B251" s="33"/>
     </row>
-    <row r="252" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="252" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B252" s="33"/>
     </row>
-    <row r="253" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="253" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B253" s="33"/>
     </row>
-    <row r="254" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="254" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B254" s="33"/>
     </row>
-    <row r="255" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="255" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B255" s="33"/>
     </row>
-    <row r="256" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="256" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B256" s="33"/>
     </row>
-    <row r="257" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="257" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B257" s="33"/>
     </row>
-    <row r="258" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="258" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B258" s="33"/>
     </row>
-    <row r="259" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="259" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B259" s="33"/>
     </row>
-    <row r="260" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="260" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B260" s="33"/>
     </row>
-    <row r="261" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="261" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B261" s="33"/>
     </row>
-    <row r="262" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="262" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B262" s="33"/>
     </row>
-    <row r="263" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="263" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B263" s="33"/>
     </row>
-    <row r="264" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="264" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B264" s="33"/>
     </row>
-    <row r="265" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="265" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B265" s="33"/>
     </row>
-    <row r="266" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="266" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B266" s="33"/>
     </row>
-    <row r="267" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="267" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B267" s="33"/>
     </row>
-    <row r="268" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="268" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B268" s="33"/>
     </row>
-    <row r="269" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="269" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B269" s="33"/>
     </row>
-    <row r="270" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="270" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B270" s="33"/>
     </row>
-    <row r="271" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="271" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B271" s="33"/>
     </row>
-    <row r="272" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="272" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B272" s="33"/>
     </row>
-    <row r="273" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="273" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B273" s="33"/>
     </row>
-    <row r="274" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="274" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B274" s="33"/>
     </row>
-    <row r="275" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="275" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B275" s="33"/>
     </row>
-    <row r="276" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="276" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B276" s="33"/>
     </row>
-    <row r="277" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="277" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B277" s="33"/>
     </row>
-    <row r="278" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="278" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B278" s="33"/>
     </row>
-    <row r="279" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="279" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B279" s="33"/>
     </row>
-    <row r="280" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="280" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B280" s="33"/>
     </row>
-    <row r="281" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="281" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B281" s="33"/>
     </row>
-    <row r="282" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="282" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B282" s="33"/>
     </row>
-    <row r="283" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="283" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B283" s="33"/>
     </row>
-    <row r="284" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="284" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B284" s="33"/>
     </row>
-    <row r="285" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="285" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B285" s="33"/>
     </row>
-    <row r="286" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="286" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B286" s="33"/>
     </row>
-    <row r="287" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="287" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B287" s="33"/>
     </row>
-    <row r="288" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="288" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B288" s="33"/>
     </row>
-    <row r="289" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="289" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B289" s="33"/>
     </row>
-    <row r="290" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="290" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B290" s="33"/>
     </row>
-    <row r="291" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="291" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B291" s="33"/>
     </row>
-    <row r="292" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="292" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B292" s="33"/>
     </row>
-    <row r="293" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="293" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B293" s="33"/>
     </row>
-    <row r="294" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="294" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B294" s="33"/>
     </row>
-    <row r="295" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="295" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B295" s="33"/>
     </row>
-    <row r="296" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="296" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B296" s="33"/>
     </row>
-    <row r="297" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="297" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B297" s="33"/>
     </row>
-    <row r="298" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="298" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B298" s="33"/>
     </row>
-    <row r="299" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="299" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B299" s="33"/>
     </row>
-    <row r="300" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="300" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B300" s="33"/>
     </row>
-    <row r="301" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="301" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B301" s="33"/>
     </row>
-    <row r="302" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="302" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B302" s="33"/>
     </row>
-    <row r="303" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="303" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B303" s="33"/>
     </row>
-    <row r="304" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="304" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B304" s="33"/>
     </row>
-    <row r="305" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="305" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B305" s="33"/>
     </row>
-    <row r="306" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="306" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B306" s="33"/>
     </row>
-    <row r="307" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="307" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B307" s="33"/>
     </row>
-    <row r="308" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="308" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B308" s="33"/>
     </row>
-    <row r="309" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="309" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B309" s="33"/>
     </row>
-    <row r="310" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="310" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B310" s="33"/>
     </row>
-    <row r="311" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="311" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B311" s="33"/>
     </row>
-    <row r="312" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="312" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B312" s="33"/>
     </row>
-    <row r="313" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="313" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B313" s="33"/>
     </row>
-    <row r="314" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="314" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B314" s="33"/>
     </row>
-    <row r="315" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="315" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B315" s="33"/>
     </row>
-    <row r="316" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="316" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B316" s="33"/>
     </row>
-    <row r="317" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="317" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B317" s="33"/>
     </row>
-    <row r="318" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="318" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B318" s="33"/>
     </row>
-    <row r="319" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="319" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B319" s="33"/>
     </row>
-    <row r="320" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="320" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B320" s="33"/>
     </row>
-    <row r="321" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="321" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B321" s="33"/>
     </row>
-    <row r="322" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="322" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B322" s="33"/>
     </row>
-    <row r="323" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="323" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B323" s="33"/>
     </row>
-    <row r="324" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="324" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B324" s="33"/>
     </row>
-    <row r="325" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="325" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B325" s="33"/>
     </row>
-    <row r="326" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="326" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B326" s="33"/>
     </row>
-    <row r="327" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="327" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B327" s="33"/>
     </row>
-    <row r="328" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="328" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B328" s="33"/>
     </row>
-    <row r="329" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="329" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B329" s="33"/>
     </row>
-    <row r="330" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="330" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B330" s="33"/>
     </row>
-    <row r="331" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="331" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B331" s="33"/>
     </row>
-    <row r="332" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="332" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B332" s="33"/>
     </row>
-    <row r="333" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="333" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B333" s="33"/>
     </row>
-    <row r="334" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="334" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B334" s="33"/>
     </row>
-    <row r="335" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="335" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B335" s="33"/>
     </row>
-    <row r="336" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="336" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B336" s="33"/>
     </row>
-    <row r="337" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="337" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B337" s="33"/>
     </row>
-    <row r="338" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="338" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B338" s="33"/>
     </row>
-    <row r="339" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="339" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B339" s="33"/>
     </row>
-    <row r="340" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="340" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B340" s="33"/>
     </row>
-    <row r="341" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="341" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B341" s="33"/>
     </row>
-    <row r="342" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="342" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B342" s="33"/>
     </row>
-    <row r="343" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="343" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B343" s="33"/>
     </row>
-    <row r="344" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="344" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B344" s="33"/>
     </row>
-    <row r="345" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="345" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B345" s="33"/>
     </row>
-    <row r="346" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="346" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B346" s="33"/>
     </row>
-    <row r="347" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="347" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B347" s="33"/>
     </row>
-    <row r="348" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="348" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B348" s="33"/>
     </row>
-    <row r="349" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="349" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B349" s="33"/>
     </row>
-    <row r="350" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="350" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B350" s="33"/>
     </row>
-    <row r="351" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="351" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B351" s="33"/>
     </row>
-    <row r="352" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="352" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B352" s="33"/>
     </row>
-    <row r="353" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="353" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B353" s="33"/>
     </row>
-    <row r="354" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="354" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B354" s="33"/>
     </row>
-    <row r="355" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="355" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B355" s="33"/>
     </row>
-    <row r="356" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="356" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B356" s="33"/>
     </row>
-    <row r="357" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="357" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B357" s="33"/>
     </row>
-    <row r="358" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="358" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B358" s="33"/>
     </row>
-    <row r="359" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="359" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B359" s="33"/>
     </row>
-    <row r="360" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="360" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B360" s="33"/>
     </row>
-    <row r="361" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="361" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B361" s="33"/>
     </row>
-    <row r="362" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="362" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B362" s="33"/>
     </row>
-    <row r="363" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="363" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B363" s="33"/>
     </row>
-    <row r="364" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="364" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B364" s="33"/>
     </row>
-    <row r="365" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="365" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B365" s="33"/>
     </row>
-    <row r="366" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="366" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B366" s="33"/>
     </row>
-    <row r="367" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="367" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B367" s="33"/>
     </row>
-    <row r="368" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="368" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B368" s="33"/>
     </row>
-    <row r="369" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="369" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B369" s="33"/>
     </row>
-    <row r="370" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="370" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B370" s="33"/>
     </row>
-    <row r="371" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="371" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B371" s="33"/>
     </row>
-    <row r="372" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="372" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B372" s="33"/>
     </row>
-    <row r="373" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="373" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B373" s="33"/>
     </row>
-    <row r="374" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="374" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B374" s="33"/>
     </row>
-    <row r="375" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="375" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B375" s="33"/>
     </row>
-    <row r="376" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="376" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B376" s="33"/>
     </row>
-    <row r="377" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="377" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B377" s="33"/>
     </row>
-    <row r="378" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="378" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B378" s="33"/>
     </row>
-    <row r="379" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="379" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B379" s="33"/>
     </row>
-    <row r="380" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="380" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B380" s="33"/>
     </row>
-    <row r="381" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="381" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B381" s="33"/>
     </row>
-    <row r="382" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="382" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B382" s="33"/>
     </row>
-    <row r="383" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="383" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B383" s="33"/>
     </row>
-    <row r="384" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="384" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B384" s="33"/>
     </row>
-    <row r="385" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="385" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B385" s="33"/>
     </row>
-    <row r="386" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="386" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B386" s="33"/>
     </row>
-    <row r="387" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="387" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B387" s="33"/>
     </row>
-    <row r="388" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="388" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B388" s="33"/>
     </row>
-    <row r="389" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="389" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B389" s="33"/>
     </row>
-    <row r="390" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="390" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B390" s="33"/>
     </row>
-    <row r="391" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="391" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B391" s="33"/>
     </row>
-    <row r="392" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="392" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B392" s="33"/>
     </row>
-    <row r="393" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="393" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B393" s="33"/>
     </row>
-    <row r="394" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="394" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B394" s="33"/>
     </row>
-    <row r="395" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="395" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B395" s="33"/>
     </row>
-    <row r="396" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="396" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B396" s="33"/>
     </row>
-    <row r="397" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="397" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B397" s="33"/>
     </row>
-    <row r="398" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="398" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B398" s="33"/>
     </row>
-    <row r="399" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="399" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B399" s="33"/>
     </row>
-    <row r="400" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="400" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B400" s="33"/>
     </row>
-    <row r="401" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="401" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B401" s="33"/>
     </row>
-    <row r="402" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="402" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B402" s="33"/>
     </row>
-    <row r="403" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="403" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B403" s="33"/>
     </row>
-    <row r="404" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="404" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B404" s="33"/>
     </row>
-    <row r="405" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="405" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B405" s="33"/>
     </row>
-    <row r="406" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="406" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B406" s="33"/>
     </row>
-    <row r="407" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="407" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B407" s="33"/>
     </row>
-    <row r="408" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="408" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B408" s="33"/>
     </row>
-    <row r="409" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="409" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B409" s="33"/>
     </row>
-    <row r="410" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="410" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B410" s="33"/>
     </row>
-    <row r="411" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="411" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B411" s="33"/>
     </row>
-    <row r="412" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="412" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B412" s="33"/>
     </row>
-    <row r="413" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="413" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B413" s="33"/>
     </row>
-    <row r="414" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="414" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B414" s="33"/>
     </row>
-    <row r="415" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="415" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B415" s="33"/>
     </row>
-    <row r="416" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="416" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B416" s="33"/>
     </row>
-    <row r="417" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="417" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B417" s="33"/>
     </row>
-    <row r="418" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="418" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B418" s="33"/>
     </row>
-    <row r="419" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="419" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B419" s="33"/>
     </row>
-    <row r="420" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="420" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B420" s="33"/>
     </row>
-    <row r="421" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="421" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B421" s="33"/>
     </row>
-    <row r="422" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="422" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B422" s="33"/>
     </row>
-    <row r="423" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="423" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B423" s="33"/>
     </row>
-    <row r="424" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="424" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B424" s="33"/>
     </row>
-    <row r="425" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="425" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B425" s="33"/>
     </row>
-    <row r="426" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="426" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B426" s="33"/>
     </row>
-    <row r="427" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="427" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B427" s="33"/>
     </row>
-    <row r="428" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="428" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B428" s="33"/>
     </row>
-    <row r="429" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="429" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B429" s="33"/>
     </row>
-    <row r="430" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="430" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B430" s="33"/>
     </row>
-    <row r="431" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="431" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B431" s="33"/>
     </row>
-    <row r="432" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="432" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B432" s="33"/>
     </row>
-    <row r="433" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="433" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B433" s="33"/>
     </row>
-    <row r="434" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="434" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B434" s="33"/>
     </row>
-    <row r="435" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="435" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B435" s="33"/>
     </row>
-    <row r="436" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="436" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B436" s="33"/>
     </row>
-    <row r="437" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="437" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B437" s="33"/>
     </row>
-    <row r="438" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="438" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B438" s="33"/>
     </row>
-    <row r="439" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="439" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B439" s="33"/>
     </row>
-    <row r="440" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="440" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B440" s="33"/>
     </row>
-    <row r="441" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="441" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B441" s="33"/>
     </row>
-    <row r="442" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="442" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B442" s="33"/>
     </row>
-    <row r="443" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="443" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B443" s="33"/>
     </row>
-    <row r="444" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="444" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B444" s="33"/>
     </row>
-    <row r="445" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="445" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B445" s="33"/>
     </row>
-    <row r="446" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="446" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B446" s="33"/>
     </row>
-    <row r="447" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="447" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B447" s="33"/>
     </row>
-    <row r="448" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="448" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B448" s="33"/>
     </row>
-    <row r="449" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="449" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B449" s="33"/>
     </row>
-    <row r="450" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="450" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B450" s="33"/>
     </row>
-    <row r="451" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="451" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B451" s="33"/>
     </row>
-    <row r="452" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="452" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B452" s="33"/>
     </row>
-    <row r="453" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="453" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B453" s="33"/>
     </row>
-    <row r="454" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="454" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B454" s="33"/>
     </row>
-    <row r="455" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="455" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B455" s="33"/>
     </row>
-    <row r="456" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="456" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B456" s="33"/>
     </row>
-    <row r="457" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="457" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B457" s="33"/>
     </row>
-    <row r="458" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="458" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B458" s="33"/>
     </row>
-    <row r="459" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="459" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B459" s="33"/>
     </row>
-    <row r="460" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="460" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B460" s="33"/>
     </row>
-    <row r="461" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="461" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B461" s="33"/>
     </row>
-    <row r="462" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="462" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B462" s="33"/>
     </row>
-    <row r="463" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="463" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B463" s="33"/>
     </row>
-    <row r="464" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="464" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B464" s="33"/>
     </row>
-    <row r="465" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="465" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B465" s="33"/>
     </row>
-    <row r="466" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="466" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B466" s="33"/>
     </row>
-    <row r="467" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="467" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B467" s="33"/>
     </row>
-    <row r="468" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="468" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B468" s="33"/>
     </row>
-    <row r="469" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="469" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B469" s="33"/>
     </row>
-    <row r="470" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="470" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B470" s="33"/>
     </row>
-    <row r="471" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="471" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B471" s="33"/>
     </row>
-    <row r="472" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="472" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B472" s="33"/>
     </row>
-    <row r="473" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="473" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B473" s="33"/>
     </row>
-    <row r="474" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="474" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B474" s="33"/>
     </row>
-    <row r="475" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="475" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B475" s="33"/>
     </row>
-    <row r="476" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="476" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B476" s="33"/>
     </row>
-    <row r="477" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="477" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B477" s="33"/>
     </row>
-    <row r="478" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="478" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B478" s="33"/>
     </row>
-    <row r="479" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="479" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B479" s="33"/>
     </row>
-    <row r="480" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="480" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B480" s="33"/>
     </row>
-    <row r="481" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="481" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B481" s="33"/>
     </row>
-    <row r="482" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="482" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B482" s="33"/>
     </row>
-    <row r="483" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="483" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B483" s="33"/>
     </row>
-    <row r="484" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="484" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B484" s="33"/>
     </row>
-    <row r="485" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="485" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B485" s="33"/>
     </row>
-    <row r="486" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="486" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B486" s="33"/>
     </row>
-    <row r="487" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="487" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B487" s="33"/>
     </row>
-    <row r="488" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="488" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B488" s="33"/>
     </row>
-    <row r="489" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="489" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B489" s="33"/>
     </row>
-    <row r="490" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="490" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B490" s="33"/>
     </row>
-    <row r="491" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="491" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B491" s="33"/>
     </row>
-    <row r="492" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="492" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B492" s="33"/>
     </row>
-    <row r="493" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="493" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B493" s="33"/>
     </row>
-    <row r="494" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="494" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B494" s="33"/>
     </row>
-    <row r="495" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="495" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B495" s="33"/>
     </row>
-    <row r="496" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="496" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B496" s="33"/>
     </row>
-    <row r="497" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="497" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B497" s="33"/>
     </row>
-    <row r="498" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="498" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B498" s="33"/>
     </row>
-    <row r="499" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="499" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B499" s="33"/>
     </row>
-    <row r="500" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="500" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B500" s="33"/>
     </row>
-    <row r="501" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="501" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B501" s="33"/>
     </row>
-    <row r="502" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="502" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B502" s="33"/>
     </row>
-    <row r="503" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="503" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B503" s="33"/>
     </row>
-    <row r="504" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="504" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B504" s="33"/>
     </row>
-    <row r="505" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="505" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B505" s="33"/>
     </row>
-    <row r="506" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="506" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B506" s="33"/>
     </row>
-    <row r="507" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="507" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B507" s="33"/>
     </row>
-    <row r="508" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="508" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B508" s="33"/>
     </row>
-    <row r="509" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="509" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B509" s="33"/>
     </row>
-    <row r="510" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="510" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B510" s="33"/>
     </row>
-    <row r="511" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="511" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B511" s="33"/>
     </row>
-    <row r="512" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="512" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B512" s="33"/>
     </row>
-    <row r="513" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="513" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B513" s="33"/>
     </row>
-    <row r="514" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="514" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B514" s="33"/>
     </row>
-    <row r="515" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="515" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B515" s="33"/>
     </row>
-    <row r="516" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="516" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B516" s="33"/>
     </row>
-    <row r="517" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="517" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B517" s="33"/>
     </row>
-    <row r="518" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="518" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B518" s="33"/>
     </row>
-    <row r="519" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="519" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B519" s="33"/>
     </row>
-    <row r="520" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="520" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B520" s="33"/>
     </row>
-    <row r="521" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="521" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B521" s="33"/>
     </row>
-    <row r="522" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="522" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B522" s="33"/>
     </row>
-    <row r="523" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="523" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B523" s="33"/>
     </row>
-    <row r="524" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="524" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B524" s="33"/>
     </row>
-    <row r="525" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="525" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B525" s="33"/>
     </row>
-    <row r="526" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="526" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B526" s="33"/>
     </row>
-    <row r="527" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="527" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B527" s="33"/>
     </row>
-    <row r="528" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="528" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B528" s="33"/>
     </row>
-    <row r="529" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="529" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B529" s="33"/>
     </row>
-    <row r="530" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="530" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B530" s="33"/>
     </row>
-    <row r="531" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="531" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B531" s="33"/>
     </row>
-    <row r="532" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="532" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B532" s="33"/>
     </row>
-    <row r="533" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="533" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B533" s="33"/>
     </row>
-    <row r="534" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="534" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B534" s="33"/>
     </row>
-    <row r="535" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="535" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B535" s="33"/>
     </row>
-    <row r="536" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="536" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B536" s="33"/>
     </row>
-    <row r="537" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="537" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B537" s="33"/>
     </row>
-    <row r="538" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="538" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B538" s="33"/>
     </row>
-    <row r="539" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="539" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B539" s="33"/>
     </row>
-    <row r="540" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="540" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B540" s="33"/>
     </row>
-    <row r="541" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="541" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B541" s="33"/>
     </row>
-    <row r="542" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="542" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B542" s="33"/>
     </row>
-    <row r="543" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="543" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B543" s="33"/>
     </row>
-    <row r="544" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="544" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B544" s="33"/>
     </row>
-    <row r="545" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="545" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B545" s="33"/>
     </row>
-    <row r="546" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="546" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B546" s="33"/>
     </row>
-    <row r="547" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="547" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B547" s="33"/>
     </row>
-    <row r="548" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="548" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B548" s="33"/>
     </row>
-    <row r="549" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="549" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B549" s="33"/>
     </row>
-    <row r="550" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="550" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B550" s="33"/>
     </row>
-    <row r="551" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="551" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B551" s="33"/>
     </row>
-    <row r="552" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="552" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B552" s="33"/>
     </row>
-    <row r="553" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="553" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B553" s="33"/>
     </row>
-    <row r="554" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="554" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B554" s="33"/>
     </row>
-    <row r="555" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="555" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B555" s="33"/>
     </row>
-    <row r="556" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="556" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B556" s="33"/>
     </row>
-    <row r="557" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="557" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B557" s="33"/>
     </row>
-    <row r="558" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="558" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B558" s="33"/>
     </row>
-    <row r="559" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="559" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B559" s="33"/>
     </row>
-    <row r="560" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="560" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B560" s="33"/>
     </row>
-    <row r="561" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="561" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B561" s="33"/>
     </row>
-    <row r="562" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="562" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B562" s="33"/>
     </row>
-    <row r="563" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="563" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B563" s="33"/>
     </row>
-    <row r="564" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="564" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B564" s="33"/>
     </row>
-    <row r="565" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="565" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B565" s="33"/>
     </row>
-    <row r="566" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="566" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B566" s="33"/>
     </row>
-    <row r="567" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="567" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B567" s="33"/>
     </row>
-    <row r="568" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="568" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B568" s="33"/>
     </row>
-    <row r="569" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="569" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B569" s="33"/>
     </row>
-    <row r="570" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="570" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B570" s="33"/>
     </row>
-    <row r="571" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="571" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B571" s="33"/>
     </row>
-    <row r="572" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="572" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B572" s="33"/>
     </row>
-    <row r="573" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="573" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B573" s="33"/>
     </row>
-    <row r="574" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="574" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B574" s="33"/>
     </row>
-    <row r="575" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="575" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B575" s="33"/>
     </row>
-    <row r="576" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="576" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B576" s="33"/>
     </row>
-    <row r="577" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="577" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B577" s="33"/>
     </row>
-    <row r="578" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="578" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B578" s="33"/>
     </row>
-    <row r="579" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="579" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B579" s="33"/>
     </row>
-    <row r="580" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="580" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B580" s="33"/>
     </row>
-    <row r="581" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="581" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B581" s="33"/>
     </row>
-    <row r="582" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="582" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B582" s="33"/>
     </row>
-    <row r="583" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="583" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B583" s="33"/>
     </row>
-    <row r="584" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="584" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B584" s="33"/>
     </row>
-    <row r="585" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="585" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B585" s="33"/>
     </row>
-    <row r="586" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="586" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B586" s="33"/>
     </row>
-    <row r="587" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="587" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B587" s="33"/>
     </row>
-    <row r="588" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="588" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B588" s="33"/>
     </row>
-    <row r="589" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="589" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B589" s="33"/>
     </row>
-    <row r="590" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="590" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B590" s="33"/>
     </row>
-    <row r="591" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="591" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B591" s="33"/>
     </row>
-    <row r="592" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="592" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B592" s="33"/>
     </row>
-    <row r="593" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="593" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B593" s="33"/>
     </row>
-    <row r="594" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="594" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B594" s="33"/>
     </row>
-    <row r="595" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="595" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B595" s="33"/>
     </row>
-    <row r="596" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="596" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B596" s="33"/>
     </row>
-    <row r="597" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="597" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B597" s="33"/>
     </row>
-    <row r="598" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="598" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B598" s="33"/>
     </row>
-    <row r="599" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="599" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B599" s="33"/>
     </row>
-    <row r="600" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="600" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B600" s="33"/>
     </row>
-    <row r="601" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="601" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B601" s="33"/>
     </row>
-    <row r="602" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="602" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B602" s="33"/>
     </row>
-    <row r="603" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="603" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B603" s="33"/>
     </row>
-    <row r="604" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="604" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B604" s="33"/>
     </row>
-    <row r="605" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="605" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B605" s="33"/>
     </row>
-    <row r="606" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="606" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B606" s="33"/>
     </row>
-    <row r="607" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="607" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B607" s="33"/>
     </row>
-    <row r="608" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="608" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B608" s="33"/>
     </row>
-    <row r="609" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="609" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B609" s="33"/>
     </row>
-    <row r="610" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="610" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B610" s="33"/>
     </row>
-    <row r="611" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="611" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B611" s="33"/>
     </row>
-    <row r="612" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="612" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B612" s="33"/>
     </row>
-    <row r="613" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="613" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B613" s="33"/>
     </row>
-    <row r="614" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="614" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B614" s="33"/>
     </row>
-    <row r="615" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="615" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B615" s="33"/>
     </row>
-    <row r="616" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="616" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B616" s="33"/>
     </row>
-    <row r="617" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="617" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B617" s="33"/>
     </row>
-    <row r="618" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="618" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B618" s="33"/>
     </row>
-    <row r="619" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="619" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B619" s="33"/>
     </row>
-    <row r="620" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="620" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B620" s="33"/>
     </row>
-    <row r="621" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="621" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B621" s="33"/>
     </row>
-    <row r="622" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="622" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B622" s="33"/>
     </row>
-    <row r="623" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="623" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B623" s="33"/>
     </row>
-    <row r="624" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="624" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B624" s="33"/>
     </row>
-    <row r="625" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="625" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B625" s="33"/>
     </row>
-    <row r="626" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="626" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B626" s="33"/>
     </row>
-    <row r="627" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="627" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B627" s="33"/>
     </row>
-    <row r="628" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="628" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B628" s="33"/>
     </row>
-    <row r="629" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="629" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B629" s="33"/>
     </row>
-    <row r="630" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="630" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B630" s="33"/>
     </row>
-    <row r="631" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="631" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B631" s="33"/>
     </row>
-    <row r="632" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="632" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B632" s="33"/>
     </row>
-    <row r="633" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="633" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B633" s="33"/>
     </row>
-    <row r="634" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="634" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B634" s="33"/>
     </row>
-    <row r="635" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="635" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B635" s="33"/>
     </row>
-    <row r="636" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="636" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B636" s="33"/>
     </row>
-    <row r="637" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="637" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B637" s="33"/>
     </row>
-    <row r="638" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="638" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B638" s="33"/>
     </row>
-    <row r="639" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="639" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B639" s="33"/>
     </row>
-    <row r="640" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="640" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B640" s="33"/>
     </row>
-    <row r="641" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="641" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B641" s="33"/>
     </row>
-    <row r="642" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="642" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B642" s="33"/>
     </row>
-    <row r="643" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="643" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B643" s="33"/>
     </row>
-    <row r="644" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="644" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B644" s="33"/>
     </row>
-    <row r="645" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="645" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B645" s="33"/>
     </row>
-    <row r="646" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="646" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B646" s="33"/>
     </row>
-    <row r="647" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="647" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B647" s="33"/>
     </row>
-    <row r="648" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="648" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B648" s="33"/>
     </row>
-    <row r="649" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="649" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B649" s="33"/>
     </row>
-    <row r="650" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="650" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B650" s="33"/>
     </row>
-    <row r="651" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="651" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B651" s="33"/>
     </row>
-    <row r="652" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="652" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B652" s="33"/>
     </row>
-    <row r="653" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="653" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B653" s="33"/>
     </row>
-    <row r="654" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="654" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B654" s="33"/>
     </row>
-    <row r="655" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="655" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B655" s="33"/>
     </row>
-    <row r="656" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="656" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B656" s="33"/>
     </row>
-    <row r="657" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="657" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B657" s="33"/>
     </row>
-    <row r="658" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="658" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B658" s="33"/>
     </row>
-    <row r="659" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="659" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B659" s="33"/>
     </row>
-    <row r="660" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="660" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B660" s="33"/>
     </row>
-    <row r="661" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="661" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B661" s="33"/>
     </row>
-    <row r="662" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="662" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B662" s="33"/>
     </row>
-    <row r="663" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="663" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B663" s="33"/>
     </row>
-    <row r="664" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="664" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B664" s="33"/>
     </row>
-    <row r="665" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="665" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B665" s="33"/>
     </row>
-    <row r="666" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="666" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B666" s="33"/>
     </row>
-    <row r="667" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="667" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B667" s="33"/>
     </row>
   </sheetData>
@@ -6336,21 +6356,21 @@
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="45"/>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="46"/>
       <c r="C1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -6361,7 +6381,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>0</v>
       </c>
@@ -6372,7 +6392,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1</v>
       </c>
@@ -6383,7 +6403,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1</v>
       </c>
@@ -6406,30 +6426,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D74D41B-283E-4F55-BA94-91EF2EF7E1E9}">
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:H25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" customWidth="1"/>
+    <col min="1" max="8" width="10.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="25" t="s">
         <v>60</v>
       </c>
@@ -6455,19 +6473,19 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="47" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="49"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="50"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="25" t="s">
         <v>68</v>
       </c>
@@ -6493,19 +6511,19 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="46" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="B7" s="46"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="25" t="s">
         <v>60</v>
       </c>
@@ -6531,19 +6549,19 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="47" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="B9" s="48"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="49"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="49"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="50"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="25" t="s">
         <v>68</v>
       </c>
@@ -6569,19 +6587,19 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="46" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="B13" s="46"/>
-      <c r="C13" s="46"/>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="46"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="47"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="47"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="25" t="s">
         <v>60</v>
       </c>
@@ -6607,19 +6625,19 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="47" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="B15" s="48"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="48"/>
-      <c r="H15" s="49"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="49"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="49"/>
+      <c r="H15" s="50"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="25" t="s">
         <v>68</v>
       </c>
@@ -6645,19 +6663,19 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="46" t="s">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="B19" s="46"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="46"/>
-      <c r="H19" s="46"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="47"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="47"/>
+      <c r="H19" s="47"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="25" t="s">
         <v>60</v>
       </c>
@@ -6683,19 +6701,19 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="47" t="s">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="B21" s="48"/>
-      <c r="C21" s="48"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="48"/>
-      <c r="H21" s="49"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="49"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="49"/>
+      <c r="H21" s="50"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="25" t="s">
         <v>68</v>
       </c>
@@ -6721,19 +6739,19 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="46" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="B25" s="46"/>
-      <c r="C25" s="46"/>
-      <c r="D25" s="46"/>
-      <c r="E25" s="46"/>
-      <c r="F25" s="46"/>
-      <c r="G25" s="46"/>
-      <c r="H25" s="46"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="47"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="47"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="47"/>
+      <c r="G25" s="47"/>
+      <c r="H25" s="47"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="6" t="s">
         <v>60</v>
       </c>
@@ -6759,7 +6777,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="24">
         <v>0</v>
       </c>
@@ -6785,7 +6803,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="6" t="s">
         <v>67</v>
       </c>
@@ -6811,19 +6829,19 @@
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="46" t="s">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="B31" s="46"/>
-      <c r="C31" s="46"/>
-      <c r="D31" s="46"/>
-      <c r="E31" s="46"/>
-      <c r="F31" s="46"/>
-      <c r="G31" s="46"/>
-      <c r="H31" s="46"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="47"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="47"/>
+      <c r="H31" s="47"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="6" t="s">
         <v>60</v>
       </c>
@@ -6849,7 +6867,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="6">
         <v>0</v>
       </c>
@@ -6862,14 +6880,14 @@
       <c r="D33" s="6">
         <v>0</v>
       </c>
-      <c r="E33" s="46" t="s">
+      <c r="E33" s="47" t="s">
         <v>62</v>
       </c>
-      <c r="F33" s="46"/>
-      <c r="G33" s="46"/>
-      <c r="H33" s="46"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F33" s="47"/>
+      <c r="G33" s="47"/>
+      <c r="H33" s="47"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="6" t="s">
         <v>67</v>
       </c>
@@ -6895,19 +6913,19 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="46" t="s">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A37" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="B37" s="46"/>
-      <c r="C37" s="46"/>
-      <c r="D37" s="46"/>
-      <c r="E37" s="46"/>
-      <c r="F37" s="46"/>
-      <c r="G37" s="46"/>
-      <c r="H37" s="46"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="47"/>
+      <c r="C37" s="47"/>
+      <c r="D37" s="47"/>
+      <c r="E37" s="47"/>
+      <c r="F37" s="47"/>
+      <c r="G37" s="47"/>
+      <c r="H37" s="47"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="20" t="s">
         <v>60</v>
       </c>
@@ -6933,33 +6951,33 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="20">
         <v>0</v>
       </c>
-      <c r="B39" s="20">
-        <v>0</v>
+      <c r="B39" s="20" t="s">
+        <v>131</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>131</v>
-      </c>
-      <c r="D39" s="20" t="s">
         <v>90</v>
       </c>
+      <c r="D39" s="6" t="s">
+        <v>82</v>
+      </c>
       <c r="E39" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="G39" s="6" t="s">
         <v>80</v>
+      </c>
+      <c r="G39" s="51" t="s">
+        <v>135</v>
       </c>
       <c r="H39" s="20" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="20" t="s">
         <v>67</v>
       </c>
@@ -6978,8 +6996,8 @@
       <c r="F40" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="G40" s="20" t="s">
-        <v>67</v>
+      <c r="G40" s="39" t="s">
+        <v>68</v>
       </c>
       <c r="H40" s="20" t="s">
         <v>68</v>
@@ -6987,18 +7005,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="A9:H9"/>
     <mergeCell ref="A37:H37"/>
     <mergeCell ref="A25:H25"/>
     <mergeCell ref="A31:H31"/>
     <mergeCell ref="E33:H33"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A7:H7"/>
-    <mergeCell ref="A13:H13"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="A21:H21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>